<commit_message>
Update Readme and Contact  Information
</commit_message>
<xml_diff>
--- a/Contact information.xlsx
+++ b/Contact information.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="180">
   <si>
     <t>ID</t>
   </si>
@@ -80,7 +80,7 @@
     <t>Journal of Experimental Psychology:  Human Perception and Performance</t>
   </si>
   <si>
-    <t>Template_1</t>
+    <t>Template_2</t>
   </si>
   <si>
     <t>Sticking together? Re-binding previous other-associated stimuli interferes with self-verification but not partner-verification</t>
@@ -446,6 +446,30 @@
   </si>
   <si>
     <t>tseng@riec.tohoku.ac.jp</t>
+  </si>
+  <si>
+    <t>The self-relevant spotlight metaphor: Self-relevant targets diminish distractor–response-binding effects</t>
+  </si>
+  <si>
+    <t>Marcel Pauly</t>
+  </si>
+  <si>
+    <t>marcel.pauly@uni-saarlande.de</t>
+  </si>
+  <si>
+    <t>Psychonomic Bulletin &amp; Review</t>
+  </si>
+  <si>
+    <t>Template_1</t>
+  </si>
+  <si>
+    <t>The self can be associated with novel faces of in-group and out-group members: A cross-cultural study</t>
+  </si>
+  <si>
+    <t>Mario Dalmaso</t>
+  </si>
+  <si>
+    <t>mario.dalmaso@unipd.it</t>
   </si>
   <si>
     <t>Paper</t>
@@ -1615,12 +1639,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:JI45"/>
+  <dimension ref="A1:JI46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="103" topLeftCell="A19" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="103" topLeftCell="A23" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="F1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="I21" sqref="I21"/>
+      <selection pane="topRight" activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -10307,10 +10331,10 @@
     </row>
     <row r="32" ht="15.5" spans="1:269">
       <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="5"/>
       <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
+      <c r="E32" s="6"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -10576,16 +10600,30 @@
       <c r="JH32" s="1"/>
       <c r="JI32" s="1"/>
     </row>
-    <row r="33" ht="15.5" spans="1:269">
+    <row r="33" ht="31" spans="1:269">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
+      <c r="C33" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G33" s="1">
+        <v>2024</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
@@ -10847,16 +10885,30 @@
       <c r="JH33" s="1"/>
       <c r="JI33" s="1"/>
     </row>
-    <row r="34" ht="15.5" spans="1:269">
+    <row r="34" ht="31" spans="1:269">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
+      <c r="C34" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G34" s="1">
+        <v>2024</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
@@ -11121,7 +11173,7 @@
     <row r="35" ht="15.5" spans="1:269">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
+      <c r="C35" s="5"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -11392,7 +11444,7 @@
     <row r="36" ht="15.5" spans="1:269">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
+      <c r="C36" s="5"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -11663,7 +11715,7 @@
     <row r="37" ht="15.5" spans="1:269">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
+      <c r="C37" s="5"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -11934,7 +11986,7 @@
     <row r="38" ht="15.5" spans="1:269">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
+      <c r="C38" s="5"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -12205,7 +12257,7 @@
     <row r="39" ht="15.5" spans="1:269">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
+      <c r="C39" s="5"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -12476,7 +12528,7 @@
     <row r="40" ht="15.5" spans="1:269">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
+      <c r="C40" s="5"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -12747,7 +12799,7 @@
     <row r="41" ht="15.5" spans="1:269">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
+      <c r="C41" s="5"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -13018,7 +13070,7 @@
     <row r="42" ht="15.5" spans="1:269">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
+      <c r="C42" s="5"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -13289,7 +13341,7 @@
     <row r="43" ht="15.5" spans="1:269">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
+      <c r="C43" s="5"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -13560,7 +13612,7 @@
     <row r="44" ht="15.5" spans="1:269">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
+      <c r="C44" s="5"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -13828,15 +13880,286 @@
       <c r="JH44" s="1"/>
       <c r="JI44" s="1"/>
     </row>
-    <row r="45" ht="15.5" spans="1:8">
+    <row r="45" ht="15.5" spans="1:269">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
+      <c r="C45" s="5"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="1"/>
+      <c r="R45" s="1"/>
+      <c r="S45" s="1"/>
+      <c r="T45" s="1"/>
+      <c r="U45" s="1"/>
+      <c r="V45" s="1"/>
+      <c r="W45" s="1"/>
+      <c r="X45" s="1"/>
+      <c r="Y45" s="1"/>
+      <c r="Z45" s="1"/>
+      <c r="AA45" s="1"/>
+      <c r="AB45" s="1"/>
+      <c r="AC45" s="1"/>
+      <c r="AD45" s="1"/>
+      <c r="AE45" s="1"/>
+      <c r="AF45" s="1"/>
+      <c r="AG45" s="1"/>
+      <c r="AH45" s="1"/>
+      <c r="AI45" s="1"/>
+      <c r="AJ45" s="1"/>
+      <c r="AK45" s="1"/>
+      <c r="AL45" s="1"/>
+      <c r="AM45" s="1"/>
+      <c r="AN45" s="1"/>
+      <c r="AO45" s="1"/>
+      <c r="AP45" s="1"/>
+      <c r="AQ45" s="1"/>
+      <c r="AR45" s="1"/>
+      <c r="AS45" s="1"/>
+      <c r="AT45" s="1"/>
+      <c r="AU45" s="1"/>
+      <c r="AV45" s="1"/>
+      <c r="AW45" s="1"/>
+      <c r="AX45" s="1"/>
+      <c r="AY45" s="1"/>
+      <c r="AZ45" s="1"/>
+      <c r="BA45" s="1"/>
+      <c r="BB45" s="1"/>
+      <c r="BC45" s="1"/>
+      <c r="BD45" s="1"/>
+      <c r="BE45" s="1"/>
+      <c r="BF45" s="1"/>
+      <c r="BG45" s="1"/>
+      <c r="BH45" s="1"/>
+      <c r="BI45" s="1"/>
+      <c r="BJ45" s="1"/>
+      <c r="BK45" s="1"/>
+      <c r="BL45" s="1"/>
+      <c r="BM45" s="1"/>
+      <c r="BN45" s="1"/>
+      <c r="BO45" s="1"/>
+      <c r="BP45" s="1"/>
+      <c r="BQ45" s="1"/>
+      <c r="BR45" s="1"/>
+      <c r="BS45" s="1"/>
+      <c r="BT45" s="1"/>
+      <c r="BU45" s="1"/>
+      <c r="BV45" s="1"/>
+      <c r="BW45" s="1"/>
+      <c r="BX45" s="1"/>
+      <c r="BY45" s="1"/>
+      <c r="BZ45" s="1"/>
+      <c r="CA45" s="1"/>
+      <c r="CB45" s="1"/>
+      <c r="CC45" s="1"/>
+      <c r="CD45" s="1"/>
+      <c r="CE45" s="1"/>
+      <c r="CF45" s="1"/>
+      <c r="CG45" s="1"/>
+      <c r="CH45" s="1"/>
+      <c r="CI45" s="1"/>
+      <c r="CJ45" s="1"/>
+      <c r="CK45" s="1"/>
+      <c r="CL45" s="1"/>
+      <c r="CM45" s="1"/>
+      <c r="CN45" s="1"/>
+      <c r="CO45" s="1"/>
+      <c r="CP45" s="1"/>
+      <c r="CQ45" s="1"/>
+      <c r="CR45" s="1"/>
+      <c r="CS45" s="1"/>
+      <c r="CT45" s="1"/>
+      <c r="CU45" s="1"/>
+      <c r="CV45" s="1"/>
+      <c r="CW45" s="1"/>
+      <c r="CX45" s="1"/>
+      <c r="CY45" s="1"/>
+      <c r="CZ45" s="1"/>
+      <c r="DA45" s="1"/>
+      <c r="DB45" s="1"/>
+      <c r="DC45" s="1"/>
+      <c r="DD45" s="1"/>
+      <c r="DE45" s="1"/>
+      <c r="DF45" s="1"/>
+      <c r="DG45" s="1"/>
+      <c r="DH45" s="1"/>
+      <c r="DI45" s="1"/>
+      <c r="DJ45" s="1"/>
+      <c r="DK45" s="1"/>
+      <c r="DL45" s="1"/>
+      <c r="DM45" s="1"/>
+      <c r="DN45" s="1"/>
+      <c r="DO45" s="1"/>
+      <c r="DP45" s="1"/>
+      <c r="DQ45" s="1"/>
+      <c r="DR45" s="1"/>
+      <c r="DS45" s="1"/>
+      <c r="DT45" s="1"/>
+      <c r="DU45" s="1"/>
+      <c r="DV45" s="1"/>
+      <c r="DW45" s="1"/>
+      <c r="DX45" s="1"/>
+      <c r="DY45" s="1"/>
+      <c r="DZ45" s="1"/>
+      <c r="EA45" s="1"/>
+      <c r="EB45" s="1"/>
+      <c r="EC45" s="1"/>
+      <c r="ED45" s="1"/>
+      <c r="EE45" s="1"/>
+      <c r="EF45" s="1"/>
+      <c r="EG45" s="1"/>
+      <c r="EH45" s="1"/>
+      <c r="EI45" s="1"/>
+      <c r="EJ45" s="1"/>
+      <c r="EK45" s="1"/>
+      <c r="EL45" s="1"/>
+      <c r="EM45" s="1"/>
+      <c r="EN45" s="1"/>
+      <c r="EO45" s="1"/>
+      <c r="EP45" s="1"/>
+      <c r="EQ45" s="1"/>
+      <c r="ER45" s="1"/>
+      <c r="ES45" s="1"/>
+      <c r="ET45" s="1"/>
+      <c r="EU45" s="1"/>
+      <c r="EV45" s="1"/>
+      <c r="EW45" s="1"/>
+      <c r="EX45" s="1"/>
+      <c r="EY45" s="1"/>
+      <c r="EZ45" s="1"/>
+      <c r="FA45" s="1"/>
+      <c r="FB45" s="1"/>
+      <c r="FC45" s="1"/>
+      <c r="FD45" s="1"/>
+      <c r="FE45" s="1"/>
+      <c r="FF45" s="1"/>
+      <c r="FG45" s="1"/>
+      <c r="FH45" s="1"/>
+      <c r="FI45" s="1"/>
+      <c r="FJ45" s="1"/>
+      <c r="FK45" s="1"/>
+      <c r="FL45" s="1"/>
+      <c r="FM45" s="1"/>
+      <c r="FN45" s="1"/>
+      <c r="FO45" s="1"/>
+      <c r="FP45" s="1"/>
+      <c r="FQ45" s="1"/>
+      <c r="FR45" s="1"/>
+      <c r="FS45" s="1"/>
+      <c r="FT45" s="1"/>
+      <c r="FU45" s="1"/>
+      <c r="FV45" s="1"/>
+      <c r="FW45" s="1"/>
+      <c r="FX45" s="1"/>
+      <c r="FY45" s="1"/>
+      <c r="FZ45" s="1"/>
+      <c r="GA45" s="1"/>
+      <c r="GB45" s="1"/>
+      <c r="GC45" s="1"/>
+      <c r="GD45" s="1"/>
+      <c r="GE45" s="1"/>
+      <c r="GF45" s="1"/>
+      <c r="GG45" s="1"/>
+      <c r="GH45" s="1"/>
+      <c r="GI45" s="1"/>
+      <c r="GJ45" s="1"/>
+      <c r="GK45" s="1"/>
+      <c r="GL45" s="1"/>
+      <c r="GM45" s="1"/>
+      <c r="GN45" s="1"/>
+      <c r="GO45" s="1"/>
+      <c r="GP45" s="1"/>
+      <c r="GQ45" s="1"/>
+      <c r="GR45" s="1"/>
+      <c r="GS45" s="1"/>
+      <c r="GT45" s="1"/>
+      <c r="GU45" s="1"/>
+      <c r="GV45" s="1"/>
+      <c r="GW45" s="1"/>
+      <c r="GX45" s="1"/>
+      <c r="GY45" s="1"/>
+      <c r="GZ45" s="1"/>
+      <c r="HA45" s="1"/>
+      <c r="HB45" s="1"/>
+      <c r="HC45" s="1"/>
+      <c r="HD45" s="1"/>
+      <c r="HE45" s="1"/>
+      <c r="HF45" s="1"/>
+      <c r="HG45" s="1"/>
+      <c r="HH45" s="1"/>
+      <c r="HI45" s="1"/>
+      <c r="HJ45" s="1"/>
+      <c r="HK45" s="1"/>
+      <c r="HL45" s="1"/>
+      <c r="HM45" s="1"/>
+      <c r="HN45" s="1"/>
+      <c r="HO45" s="1"/>
+      <c r="HP45" s="1"/>
+      <c r="HQ45" s="1"/>
+      <c r="HR45" s="1"/>
+      <c r="HS45" s="1"/>
+      <c r="HT45" s="1"/>
+      <c r="HU45" s="1"/>
+      <c r="HV45" s="1"/>
+      <c r="HW45" s="1"/>
+      <c r="HX45" s="1"/>
+      <c r="HY45" s="1"/>
+      <c r="HZ45" s="1"/>
+      <c r="IA45" s="1"/>
+      <c r="IB45" s="1"/>
+      <c r="IC45" s="1"/>
+      <c r="ID45" s="1"/>
+      <c r="IE45" s="1"/>
+      <c r="IF45" s="1"/>
+      <c r="IG45" s="1"/>
+      <c r="IH45" s="1"/>
+      <c r="II45" s="1"/>
+      <c r="IJ45" s="1"/>
+      <c r="IK45" s="1"/>
+      <c r="IL45" s="1"/>
+      <c r="IM45" s="1"/>
+      <c r="IN45" s="1"/>
+      <c r="IO45" s="1"/>
+      <c r="IP45" s="1"/>
+      <c r="IQ45" s="1"/>
+      <c r="IR45" s="1"/>
+      <c r="IS45" s="1"/>
+      <c r="IT45" s="1"/>
+      <c r="IU45" s="1"/>
+      <c r="IV45" s="1"/>
+      <c r="IW45" s="1"/>
+      <c r="IX45" s="1"/>
+      <c r="IY45" s="1"/>
+      <c r="IZ45" s="1"/>
+      <c r="JA45" s="1"/>
+      <c r="JB45" s="1"/>
+      <c r="JC45" s="1"/>
+      <c r="JD45" s="1"/>
+      <c r="JE45" s="1"/>
+      <c r="JF45" s="1"/>
+      <c r="JG45" s="1"/>
+      <c r="JH45" s="1"/>
+      <c r="JI45" s="1"/>
+    </row>
+    <row r="46" ht="15.5" spans="1:8">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
     </row>
   </sheetData>
   <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:H29" etc:filterBottomFollowUsedRange="0">
@@ -13863,6 +14186,8 @@
     <hyperlink ref="E28" r:id="rId13" display="lfuentes@um.es"/>
     <hyperlink ref="E31" r:id="rId14" display="tseng@riec.tohoku.ac.jp"/>
     <hyperlink ref="E21" r:id="rId15" display="wentura@mx.uni-saarland.de"/>
+    <hyperlink ref="E33" r:id="rId16" display="marcel.pauly@uni-saarlande.de"/>
+    <hyperlink ref="E34" r:id="rId17" display="mario.dalmaso@unipd.it"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -13889,19 +14214,19 @@
   <sheetData>
     <row r="1" ht="15.5" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -13909,19 +14234,19 @@
     </row>
     <row r="2" ht="15.5" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B2" s="1">
         <v>2019</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="E2" s="3">
         <v>2019</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="H2" s="1">
         <v>2019</v>
@@ -13929,19 +14254,19 @@
     </row>
     <row r="3" ht="15.5" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B3" s="1">
         <v>2019</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="E3" s="3">
         <v>2020</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="H3" s="1">
         <v>2019</v>
@@ -13949,19 +14274,19 @@
     </row>
     <row r="4" ht="15.5" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B4" s="1">
         <v>2019</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="E4" s="3">
         <v>2020</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="H4" s="1">
         <v>2019</v>
@@ -13969,19 +14294,19 @@
     </row>
     <row r="5" ht="15.5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B5" s="1">
         <v>2019</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="E5" s="3">
         <v>2020</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="H5" s="1">
         <v>2019</v>
@@ -13989,19 +14314,19 @@
     </row>
     <row r="6" ht="15.5" hidden="1" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B6" s="1">
         <v>2020</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="E6" s="3">
         <v>2020</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="H6" s="1">
         <v>2020</v>
@@ -14009,19 +14334,19 @@
     </row>
     <row r="7" ht="15.5" hidden="1" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="B7" s="1">
         <v>2020</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="E7" s="3">
         <v>2019</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="H7" s="1">
         <v>2020</v>
@@ -14029,19 +14354,19 @@
     </row>
     <row r="8" ht="15.5" hidden="1" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="B8" s="1">
         <v>2020</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E8" s="3">
         <v>2018</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="H8" s="1">
         <v>2020</v>
@@ -14049,19 +14374,19 @@
     </row>
     <row r="9" ht="15.5" hidden="1" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="B9" s="1">
         <v>2021</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="E9" s="3">
         <v>2021</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="H9" s="1">
         <v>2021</v>
@@ -14069,19 +14394,19 @@
     </row>
     <row r="10" ht="15.5" hidden="1" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="B10" s="1">
         <v>2020</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="E10" s="3">
         <v>2021</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="H10" s="1">
         <v>2020</v>
@@ -14089,19 +14414,19 @@
     </row>
     <row r="11" ht="15.5" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="B11" s="1">
         <v>2020</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="E11" s="3">
         <v>2022</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="H11" s="1">
         <v>2020</v>
@@ -14109,19 +14434,19 @@
     </row>
     <row r="12" ht="15.5" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="B12" s="1">
         <v>2020</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="E12" s="3">
         <v>2021</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="H12" s="1">
         <v>2020</v>
@@ -14129,19 +14454,19 @@
     </row>
     <row r="13" ht="15.5" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="B13" s="1">
         <v>2019</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="E13" s="3">
         <v>2023</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="H13" s="1">
         <v>2019</v>
@@ -14149,19 +14474,19 @@
     </row>
     <row r="14" ht="15.5" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="B14" s="1">
         <v>2019</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="E14" s="3">
         <v>2023</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="H14" s="1">
         <v>2019</v>
@@ -14169,19 +14494,19 @@
     </row>
     <row r="15" ht="15.5" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="B15" s="1">
         <v>2018</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="E15" s="3">
         <v>2014</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="H15" s="1">
         <v>2018</v>
@@ -14189,19 +14514,19 @@
     </row>
     <row r="16" ht="15.5" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="B16" s="1">
         <v>2018</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="E16" s="3">
         <v>2015</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="H16" s="1">
         <v>2018</v>
@@ -14209,19 +14534,19 @@
     </row>
     <row r="17" ht="15.5" hidden="1" spans="1:8">
       <c r="A17" s="1" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="B17" s="1">
         <v>2021</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="E17" s="3">
         <v>2014</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="H17" s="1">
         <v>2021</v>
@@ -14229,19 +14554,19 @@
     </row>
     <row r="18" ht="15.5" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="B18" s="1">
         <v>2021</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="E18" s="3">
         <v>2023</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="H18" s="1">
         <v>2021</v>
@@ -14249,19 +14574,19 @@
     </row>
     <row r="19" ht="15.5" spans="1:8">
       <c r="A19" s="1" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="B19" s="1">
         <v>2021</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="E19" s="3">
         <v>2023</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="H19" s="1">
         <v>2021</v>
@@ -14269,19 +14594,19 @@
     </row>
     <row r="20" ht="15.5" spans="1:8">
       <c r="A20" s="1" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="B20" s="1">
         <v>2021</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="E20" s="3">
         <v>2021</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="H20" s="1">
         <v>2021</v>
@@ -14289,19 +14614,19 @@
     </row>
     <row r="21" ht="15.5" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="B21" s="1">
         <v>2022</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="E21" s="3">
         <v>2023</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="H21" s="1">
         <v>2022</v>
@@ -14309,19 +14634,19 @@
     </row>
     <row r="22" ht="15.5" spans="1:8">
       <c r="A22" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="B22" s="1">
         <v>2022</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="E22" s="3">
         <v>2022</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="H22" s="1">
         <v>2022</v>
@@ -14329,19 +14654,19 @@
     </row>
     <row r="23" ht="15.5" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="B23" s="1">
         <v>2022</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="E23" s="3">
         <v>2022</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="H23" s="1">
         <v>2022</v>
@@ -14349,19 +14674,19 @@
     </row>
     <row r="24" ht="15.5" hidden="1" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="B24" s="1">
         <v>2021</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="E24" s="3">
         <v>2020</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="H24" s="1">
         <v>2021</v>
@@ -14369,19 +14694,19 @@
     </row>
     <row r="25" ht="15.5" hidden="1" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B25" s="1">
         <v>2023</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="E25" s="3">
         <v>2023</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="H25" s="1">
         <v>2023</v>
@@ -14389,19 +14714,19 @@
     </row>
     <row r="26" ht="15.5" hidden="1" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="B26" s="1">
         <v>2023</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="H26" s="1">
         <v>2023</v>
@@ -14409,13 +14734,13 @@
     </row>
     <row r="27" ht="15.5" hidden="1" spans="1:8">
       <c r="A27" s="1" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="B27" s="1">
         <v>2014</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="H27" s="1">
         <v>2014</v>
@@ -14423,13 +14748,13 @@
     </row>
     <row r="28" ht="15.5" spans="1:8">
       <c r="A28" s="1" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="B28" s="1">
         <v>2015</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="H28" s="1">
         <v>2015</v>
@@ -14437,13 +14762,13 @@
     </row>
     <row r="29" ht="15.5" spans="1:8">
       <c r="A29" s="1" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="B29" s="1">
         <v>2015</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="H29" s="1">
         <v>2015</v>
@@ -14451,13 +14776,13 @@
     </row>
     <row r="30" ht="15.5" spans="1:8">
       <c r="A30" s="1" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="B30" s="1">
         <v>2014</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="H30" s="1">
         <v>2014</v>
@@ -14465,13 +14790,13 @@
     </row>
     <row r="31" ht="15.5" spans="1:8">
       <c r="A31" s="1" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="B31" s="1">
         <v>2014</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="H31" s="1">
         <v>2014</v>
@@ -14479,13 +14804,13 @@
     </row>
     <row r="32" ht="15.5" spans="1:8">
       <c r="A32" s="1" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="B32" s="1">
         <v>2014</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="H32" s="1">
         <v>2014</v>
@@ -14493,13 +14818,13 @@
     </row>
     <row r="33" ht="15.5" spans="1:8">
       <c r="A33" s="1" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="B33" s="1">
         <v>2014</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="H33" s="1">
         <v>2014</v>
@@ -14507,13 +14832,13 @@
     </row>
     <row r="34" ht="15.5" hidden="1" spans="1:8">
       <c r="A34" s="1" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="B34" s="1">
         <v>2023</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="H34" s="1">
         <v>2023</v>
@@ -14521,13 +14846,13 @@
     </row>
     <row r="35" ht="15.5" hidden="1" spans="1:8">
       <c r="A35" s="1" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="B35" s="1">
         <v>2023</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="H35" s="1">
         <v>2023</v>
@@ -14535,13 +14860,13 @@
     </row>
     <row r="36" ht="15.5" hidden="1" spans="1:8">
       <c r="A36" s="1" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B36" s="1">
         <v>2021</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="H36" s="1">
         <v>2021</v>
@@ -14549,13 +14874,13 @@
     </row>
     <row r="37" ht="15.5" hidden="1" spans="1:8">
       <c r="A37" s="1" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="B37" s="1">
         <v>2023</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="H37" s="1">
         <v>2023</v>
@@ -14563,13 +14888,13 @@
     </row>
     <row r="38" ht="15.5" spans="1:8">
       <c r="A38" s="1" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="B38" s="1">
         <v>2022</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="H38" s="1">
         <v>2022</v>
@@ -14577,13 +14902,13 @@
     </row>
     <row r="39" ht="15.5" spans="1:8">
       <c r="A39" s="1" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="B39" s="1">
         <v>2022</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="H39" s="1">
         <v>2022</v>
@@ -14591,13 +14916,13 @@
     </row>
     <row r="40" ht="15.5" hidden="1" spans="1:8">
       <c r="A40" s="1" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="B40" s="1">
         <v>2022</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="H40" s="1">
         <v>2022</v>
@@ -14605,13 +14930,13 @@
     </row>
     <row r="41" ht="15.5" spans="1:8">
       <c r="A41" s="1" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B41" s="1">
         <v>2020</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="H41" s="1">
         <v>2020</v>
@@ -14619,13 +14944,13 @@
     </row>
     <row r="42" ht="15.5" spans="1:8">
       <c r="A42" s="1" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B42" s="1">
         <v>2020</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="H42" s="1">
         <v>2020</v>
@@ -14633,13 +14958,13 @@
     </row>
     <row r="43" ht="15.5" spans="1:8">
       <c r="A43" s="1" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B43" s="1">
         <v>2020</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="H43" s="1">
         <v>2020</v>
@@ -14647,13 +14972,13 @@
     </row>
     <row r="44" ht="15.5" spans="1:8">
       <c r="A44" s="1" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="B44" s="1">
         <v>2023</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="H44" s="1">
         <v>2023</v>
@@ -14661,13 +14986,13 @@
     </row>
     <row r="45" ht="15.5" spans="1:8">
       <c r="A45" s="1" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="B45" s="1">
         <v>2023</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="H45" s="1">
         <v>2023</v>
@@ -14675,13 +15000,13 @@
     </row>
     <row r="46" ht="15.5" spans="1:8">
       <c r="A46" s="1" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="B46" s="1">
         <v>2023</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="H46" s="1">
         <v>2023</v>
@@ -14689,13 +15014,13 @@
     </row>
     <row r="47" ht="15.5" spans="1:8">
       <c r="A47" s="1" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B47" s="1">
         <v>2021</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="H47" s="1">
         <v>2021</v>
@@ -14703,13 +15028,13 @@
     </row>
     <row r="48" ht="15.5" spans="1:8">
       <c r="A48" s="1" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B48" s="1">
         <v>2021</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="H48" s="1">
         <v>2021</v>
@@ -14717,13 +15042,13 @@
     </row>
     <row r="49" ht="15.5" spans="1:8">
       <c r="A49" s="1" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B49" s="1">
         <v>2021</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="H49" s="1">
         <v>2021</v>
@@ -14731,13 +15056,13 @@
     </row>
     <row r="50" ht="15.5" hidden="1" spans="1:8">
       <c r="A50" s="1" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="B50" s="1">
         <v>2023</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="H50" s="1">
         <v>2023</v>
@@ -14745,13 +15070,13 @@
     </row>
     <row r="51" ht="15.5" hidden="1" spans="1:8">
       <c r="A51" s="1" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="B51" s="1">
         <v>2024</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="H51" s="1">
         <v>2024</v>
@@ -14759,13 +15084,13 @@
     </row>
     <row r="52" ht="15.5" hidden="1" spans="1:8">
       <c r="A52" s="1" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="B52" s="1">
         <v>2024</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="H52" s="1">
         <v>2024</v>
@@ -14897,13 +15222,13 @@
   <sheetData>
     <row r="1" ht="15.5" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="C1" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
@@ -14911,7 +15236,7 @@
     </row>
     <row r="2" ht="15.5" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B2" s="1">
         <v>96</v>
@@ -14925,7 +15250,7 @@
     </row>
     <row r="3" ht="15.5" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B3" s="1">
         <v>96</v>
@@ -14939,7 +15264,7 @@
     </row>
     <row r="4" ht="15.5" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B4" s="1">
         <v>96</v>
@@ -14953,7 +15278,7 @@
     </row>
     <row r="5" ht="15.5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B5" s="1">
         <v>80</v>
@@ -14967,7 +15292,7 @@
     </row>
     <row r="6" ht="15.5" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B6" s="1">
         <v>240</v>
@@ -14981,7 +15306,7 @@
     </row>
     <row r="7" ht="15.5" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="B7" s="1">
         <v>312</v>
@@ -14995,7 +15320,7 @@
     </row>
     <row r="8" ht="15.5" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="B8" s="1">
         <v>100</v>
@@ -15009,7 +15334,7 @@
     </row>
     <row r="9" ht="15.5" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="B9" s="1">
         <v>960</v>
@@ -15023,7 +15348,7 @@
     </row>
     <row r="10" ht="15.5" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="B10" s="1">
         <v>192</v>
@@ -15037,7 +15362,7 @@
     </row>
     <row r="11" ht="15.5" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="B11" s="1">
         <v>144</v>
@@ -15051,7 +15376,7 @@
     </row>
     <row r="12" ht="15.5" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="B12" s="1">
         <v>100</v>
@@ -15065,7 +15390,7 @@
     </row>
     <row r="13" ht="15.5" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="B13" s="1">
         <v>144</v>
@@ -15079,7 +15404,7 @@
     </row>
     <row r="14" ht="15.5" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="B14" s="1">
         <v>672</v>
@@ -15093,7 +15418,7 @@
     </row>
     <row r="15" ht="15.5" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="B15" s="1">
         <v>672</v>
@@ -15107,7 +15432,7 @@
     </row>
     <row r="16" ht="15.5" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="B16" s="1">
         <v>360</v>
@@ -15121,7 +15446,7 @@
     </row>
     <row r="17" ht="15.5" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="B17" s="1">
         <v>360</v>
@@ -15135,7 +15460,7 @@
     </row>
     <row r="18" ht="15.5" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="B18" s="1">
         <v>360</v>
@@ -15149,7 +15474,7 @@
     </row>
     <row r="19" ht="15.5" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="B19" s="1">
         <v>360</v>
@@ -15163,7 +15488,7 @@
     </row>
     <row r="20" ht="15.5" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="B20" s="1">
         <v>360</v>
@@ -15177,7 +15502,7 @@
     </row>
     <row r="21" ht="15.5" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="B21" s="1">
         <v>360</v>
@@ -15191,7 +15516,7 @@
     </row>
     <row r="22" ht="15.5" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="B22" s="1">
         <v>128</v>
@@ -15205,7 +15530,7 @@
     </row>
     <row r="23" ht="15.5" spans="1:4">
       <c r="A23" s="1" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="B23" s="1">
         <v>240</v>
@@ -15219,7 +15544,7 @@
     </row>
     <row r="24" ht="15.5" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="B24" s="1">
         <v>240</v>
@@ -15233,7 +15558,7 @@
     </row>
     <row r="25" ht="15.5" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="B25" s="1">
         <v>200</v>
@@ -15247,7 +15572,7 @@
     </row>
     <row r="26" ht="15.5" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="B26" s="1">
         <v>400</v>
@@ -15261,7 +15586,7 @@
     </row>
     <row r="27" ht="15.5" spans="1:4">
       <c r="A27" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="B27" s="1">
         <v>400</v>
@@ -15275,7 +15600,7 @@
     </row>
     <row r="28" ht="15.5" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="B28" s="1">
         <v>360</v>
@@ -15289,7 +15614,7 @@
     </row>
     <row r="29" ht="15.5" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B29" s="1">
         <v>64</v>
@@ -15303,7 +15628,7 @@
     </row>
     <row r="30" ht="15.5" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="B30" s="1">
         <v>90</v>
@@ -15317,7 +15642,7 @@
     </row>
     <row r="31" ht="15.5" spans="1:4">
       <c r="A31" s="1" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="B31" s="1">
         <v>40</v>
@@ -15331,7 +15656,7 @@
     </row>
     <row r="32" ht="15.5" spans="1:4">
       <c r="A32" s="1" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="B32" s="1">
         <v>40</v>
@@ -15345,7 +15670,7 @@
     </row>
     <row r="33" ht="15.5" spans="1:4">
       <c r="A33" s="1" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="B33" s="1">
         <v>40</v>
@@ -15359,7 +15684,7 @@
     </row>
     <row r="34" ht="15.5" spans="1:4">
       <c r="A34" s="1" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="B34" s="1">
         <v>60</v>
@@ -15373,7 +15698,7 @@
     </row>
     <row r="35" ht="15.5" spans="1:4">
       <c r="A35" s="1" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="B35" s="1">
         <v>60</v>
@@ -15387,7 +15712,7 @@
     </row>
     <row r="36" ht="15.5" spans="1:4">
       <c r="A36" s="1" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="B36" s="1">
         <v>60</v>
@@ -15401,7 +15726,7 @@
     </row>
     <row r="37" ht="15.5" spans="1:4">
       <c r="A37" s="1" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="B37" s="1">
         <v>60</v>
@@ -15415,7 +15740,7 @@
     </row>
     <row r="38" ht="15.5" spans="1:4">
       <c r="A38" s="1" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="B38" s="1">
         <v>240</v>
@@ -15429,7 +15754,7 @@
     </row>
     <row r="39" ht="15.5" spans="1:4">
       <c r="A39" s="1" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="B39" s="1">
         <v>60</v>
@@ -15443,7 +15768,7 @@
     </row>
     <row r="40" ht="15.5" spans="1:4">
       <c r="A40" s="1" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B40" s="1">
         <v>360</v>
@@ -15457,7 +15782,7 @@
     </row>
     <row r="41" ht="15.5" spans="1:4">
       <c r="A41" s="1" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="B41" s="1">
         <v>300</v>
@@ -15471,7 +15796,7 @@
     </row>
     <row r="42" ht="15.5" spans="1:4">
       <c r="A42" s="1" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="B42" s="1">
         <v>240</v>
@@ -15485,7 +15810,7 @@
     </row>
     <row r="43" ht="15.5" spans="1:4">
       <c r="A43" s="1" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="B43" s="1">
         <v>240</v>
@@ -15499,7 +15824,7 @@
     </row>
     <row r="44" ht="15.5" spans="1:4">
       <c r="A44" s="1" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="B44" s="1">
         <v>360</v>
@@ -15513,7 +15838,7 @@
     </row>
     <row r="45" ht="15.5" spans="1:4">
       <c r="A45" s="1" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B45" s="1">
         <v>360</v>
@@ -15527,7 +15852,7 @@
     </row>
     <row r="46" ht="15.5" spans="1:4">
       <c r="A46" s="1" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B46" s="1">
         <v>360</v>
@@ -15541,7 +15866,7 @@
     </row>
     <row r="47" ht="15.5" spans="1:4">
       <c r="A47" s="1" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B47" s="1">
         <v>360</v>
@@ -15555,7 +15880,7 @@
     </row>
     <row r="48" ht="15.5" spans="1:4">
       <c r="A48" s="1" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="B48" s="1">
         <v>96</v>
@@ -15569,7 +15894,7 @@
     </row>
     <row r="49" ht="15.5" spans="1:4">
       <c r="A49" s="1" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B49" s="1">
         <v>320</v>
@@ -15583,7 +15908,7 @@
     </row>
     <row r="50" ht="15.5" spans="1:4">
       <c r="A50" s="1" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="B50" s="1">
         <v>960</v>
@@ -15597,7 +15922,7 @@
     </row>
     <row r="51" ht="15.5" spans="1:4">
       <c r="A51" s="1" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="B51" s="1">
         <v>240</v>
@@ -15611,7 +15936,7 @@
     </row>
     <row r="52" ht="15.5" spans="1:4">
       <c r="A52" s="1" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="B52" s="1">
         <v>360</v>

</xml_diff>

<commit_message>
Update Code in Compute SDE
</commit_message>
<xml_diff>
--- a/Contact information.xlsx
+++ b/Contact information.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="255">
   <si>
     <t>ID</t>
   </si>
@@ -409,6 +409,9 @@
     <t>Orellana-Corrales_2021_EP</t>
   </si>
   <si>
+    <t>√√</t>
+  </si>
+  <si>
     <t>More or less of me and you: self-relevance augments the effects of item probability on stimulus prioritization</t>
   </si>
   <si>
@@ -516,6 +519,10 @@
     <t>The oscillatory fingerprints of self-prioritization: Novel markers in spectral EEG for self-relevant processing</t>
   </si>
   <si>
+    <t>Céline C. Haciahmet,Marius Golubickis
+,Sarah Schäfer,Christian Frings,Bernhard Pastötter</t>
+  </si>
+  <si>
     <t>Bernhard Pastötter</t>
   </si>
   <si>
@@ -542,6 +549,9 @@
     <t>Self-processing in relation to emotion and reward processing in depression.</t>
   </si>
   <si>
+    <t>Catherine Hobbs,Jie Sui,David Kesslerc,Marcus R Munafò,Katherine S Button</t>
+  </si>
+  <si>
     <t>Catherine Hobbs</t>
   </si>
   <si>
@@ -563,6 +573,9 @@
     <t>The roles of the LpSTS and DLPFC in self-prioritization: A transcranial magnetic stimulation study</t>
   </si>
   <si>
+    <t>Qiongdan Liang,Bozhen Zhang,Sinan Fu,Jie Sui,Fei Wang</t>
+  </si>
+  <si>
     <t>Fei Wang</t>
   </si>
   <si>
@@ -593,7 +606,13 @@
     <t>No Trial-leve data</t>
   </si>
   <si>
+    <t>×</t>
+  </si>
+  <si>
     <t>Towards The Boundaries of Self-Prioritization: Associating The Self With Asymmetric Shapes Disrupts The Self-Prioritization Effect</t>
+  </si>
+  <si>
+    <t>Michele Vicovaro,Mario Dalmaso,Marco Bertamini</t>
   </si>
   <si>
     <t>Michele Vicovaro</t>
@@ -629,6 +648,9 @@
     <t>How selves difer within and across cognitive domains: self-prioritisation, self-concept, and psychiatric traits</t>
   </si>
   <si>
+    <t>Kelsey Perrykkad,Jakob Hohwy</t>
+  </si>
+  <si>
     <t>Kelsey Perrykkad</t>
   </si>
   <si>
@@ -650,6 +672,9 @@
     <t>Self‑prioritization depends on assumed task‑relevance of self‑association</t>
   </si>
   <si>
+    <t>Mateusz Woźniak,Guenther Knoblich</t>
+  </si>
+  <si>
     <t>https://osf.io/35wp9</t>
   </si>
   <si>
@@ -657,6 +682,9 @@
   </si>
   <si>
     <t>Decoding individual differences in self-prioritization from the resting-state functional connectome</t>
+  </si>
+  <si>
+    <t>Yongfa Zhang,Fei Wang,Jie Sui</t>
   </si>
   <si>
     <t>https://osf.io/hbrus/?view_only=98b2095f72e64fd382fc0d33de3f4497</t>
@@ -1486,7 +1514,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1528,9 +1556,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1855,13 +1880,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr filterMode="1"/>
+  <sheetPr/>
   <dimension ref="A1:JN46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" zoomScaleSheetLayoutView="70" topLeftCell="A9" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" zoomScaleSheetLayoutView="70" topLeftCell="A19" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="O37" sqref="O37"/>
+      <selection pane="topRight" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1870,13 +1895,13 @@
     <col min="2" max="2" width="16.9166666666667" customWidth="1"/>
     <col min="3" max="3" width="20.6666666666667" customWidth="1"/>
     <col min="4" max="4" width="55.8333333333333" customWidth="1"/>
-    <col min="5" max="5" width="52.0833333333333" customWidth="1"/>
-    <col min="6" max="6" width="24.5833333333333" customWidth="1"/>
-    <col min="7" max="7" width="40.0833333333333" customWidth="1"/>
-    <col min="8" max="8" width="27.55" customWidth="1"/>
-    <col min="9" max="9" width="23.4166666666667" customWidth="1"/>
-    <col min="10" max="10" width="9" customWidth="1"/>
-    <col min="11" max="11" width="67.0833333333333" customWidth="1"/>
+    <col min="5" max="5" width="55" customWidth="1"/>
+    <col min="6" max="6" width="24.5833333333333" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="40.0833333333333" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="27.55" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="23.4166666666667" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="9" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="67.0833333333333" hidden="1" customWidth="1"/>
     <col min="12" max="13" width="34.125" customWidth="1"/>
     <col min="15" max="16" width="8.75" customWidth="1"/>
     <col min="17" max="17" width="75.5" customWidth="1"/>
@@ -1943,7 +1968,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" ht="15.5" hidden="1" spans="1:274">
+    <row r="2" ht="15.5" spans="1:274">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2237,7 +2262,7 @@
       <c r="JM2" s="2"/>
       <c r="JN2" s="2"/>
     </row>
-    <row r="3" ht="31" hidden="1" spans="1:274">
+    <row r="3" ht="31" spans="1:274">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2539,7 +2564,7 @@
       <c r="JM3" s="2"/>
       <c r="JN3" s="2"/>
     </row>
-    <row r="4" ht="31" hidden="1" spans="1:274">
+    <row r="4" ht="31" spans="1:274">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3141,7 +3166,7 @@
       <c r="JM5" s="2"/>
       <c r="JN5" s="2"/>
     </row>
-    <row r="6" ht="31" hidden="1" spans="1:274">
+    <row r="6" ht="31" spans="1:274">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3437,7 +3462,7 @@
       <c r="JM6" s="2"/>
       <c r="JN6" s="2"/>
     </row>
-    <row r="7" ht="31" hidden="1" spans="1:274">
+    <row r="7" ht="31" spans="1:274">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -4667,7 +4692,7 @@
       <c r="JM10" s="2"/>
       <c r="JN10" s="2"/>
     </row>
-    <row r="11" ht="15.5" hidden="1" spans="1:274">
+    <row r="11" ht="15.5" spans="1:274">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -5273,7 +5298,7 @@
       <c r="JM12" s="2"/>
       <c r="JN12" s="2"/>
     </row>
-    <row r="13" ht="31" hidden="1" spans="1:274">
+    <row r="13" ht="31" spans="1:274">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -5312,7 +5337,7 @@
         <v>50</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>26</v>
+        <v>117</v>
       </c>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
@@ -5575,7 +5600,7 @@
       <c r="JM13" s="2"/>
       <c r="JN13" s="2"/>
     </row>
-    <row r="14" ht="46.5" hidden="1" spans="1:274">
+    <row r="14" ht="46.5" spans="1:274">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -5584,37 +5609,37 @@
         <v>26</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J14" s="2">
         <v>2022</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>50</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>26</v>
+        <v>117</v>
       </c>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
@@ -5886,34 +5911,34 @@
         <v>26</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>46</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="J15" s="2">
         <v>2021</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="N15" s="6" t="s">
         <v>26</v>
@@ -5925,7 +5950,7 @@
         <v>26</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
@@ -6194,31 +6219,31 @@
         <v>26</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J16" s="2">
         <v>2023</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>41</v>
@@ -6227,7 +6252,7 @@
         <v>26</v>
       </c>
       <c r="O16" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="P16" s="2" t="s">
         <v>26</v>
@@ -6502,10 +6527,10 @@
         <v>26</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>36</v>
@@ -6514,7 +6539,7 @@
         <v>37</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>39</v>
@@ -6524,7 +6549,7 @@
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>41</v>
@@ -6533,7 +6558,7 @@
         <v>26</v>
       </c>
       <c r="O17" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="P17" s="2" t="s">
         <v>26</v>
@@ -6810,29 +6835,31 @@
         <v>26</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="E18" s="4"/>
+        <v>147</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>148</v>
+      </c>
       <c r="F18" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="J18" s="2">
         <v>2023</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>83</v>
@@ -6847,7 +6874,7 @@
         <v>26</v>
       </c>
       <c r="Q18" s="4" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
@@ -7107,7 +7134,7 @@
       <c r="JM18" s="2"/>
       <c r="JN18" s="2"/>
     </row>
-    <row r="19" ht="31" hidden="1" spans="1:274">
+    <row r="19" ht="31" spans="1:274">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -7116,35 +7143,37 @@
         <v>26</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="E19" s="4"/>
+        <v>156</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>157</v>
+      </c>
       <c r="F19" s="2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="J19" s="2">
         <v>2023</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>50</v>
       </c>
       <c r="N19" s="6" t="s">
-        <v>26</v>
+        <v>117</v>
       </c>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
@@ -7416,20 +7445,22 @@
         <v>26</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="E20" s="6"/>
+        <v>164</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>165</v>
+      </c>
       <c r="F20" s="2" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="J20" s="2">
         <v>2021</v>
@@ -7438,7 +7469,7 @@
         <v>48</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>50</v>
@@ -7447,7 +7478,7 @@
         <v>26</v>
       </c>
       <c r="O20" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="P20" s="2" t="s">
         <v>26</v>
@@ -7713,7 +7744,7 @@
       <c r="JM20" s="2"/>
       <c r="JN20" s="2"/>
     </row>
-    <row r="21" ht="31" hidden="1" spans="1:274">
+    <row r="21" ht="31" spans="1:274">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -7722,18 +7753,18 @@
         <v>26</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="2" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H21" s="9"/>
       <c r="I21" s="9" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="J21" s="2">
         <v>2023</v>
@@ -7743,10 +7774,10 @@
       </c>
       <c r="L21" s="2"/>
       <c r="M21" s="2" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="N21" s="6" t="s">
-        <v>26</v>
+        <v>176</v>
       </c>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
@@ -8020,29 +8051,31 @@
         <v>26</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="E22" s="4"/>
+        <v>177</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>178</v>
+      </c>
       <c r="F22" s="2" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="J22" s="2">
         <v>2022</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="M22" s="2" t="s">
         <v>83</v>
@@ -8057,13 +8090,13 @@
         <v>26</v>
       </c>
       <c r="Q22" s="4" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="R22" s="4" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="S22" s="4" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
@@ -8321,7 +8354,7 @@
       <c r="JM22" s="2"/>
       <c r="JN22" s="2"/>
     </row>
-    <row r="23" ht="31" hidden="1" spans="1:274">
+    <row r="23" ht="31" spans="1:274">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -8332,35 +8365,37 @@
         <v>26</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="E23" s="4"/>
+        <v>188</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>189</v>
+      </c>
       <c r="F23" s="10" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="J23" s="2">
         <v>2022</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>83</v>
       </c>
       <c r="N23" s="6" t="s">
-        <v>26</v>
+        <v>117</v>
       </c>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
@@ -8634,9 +8669,11 @@
         <v>26</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="E24" s="4"/>
+        <v>196</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>197</v>
+      </c>
       <c r="F24" s="2" t="s">
         <v>87</v>
       </c>
@@ -8644,7 +8681,7 @@
         <v>88</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>90</v>
@@ -8653,10 +8690,10 @@
         <v>2022</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>83</v>
@@ -8938,29 +8975,31 @@
         <v>26</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="E25" s="6"/>
+        <v>200</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>201</v>
+      </c>
       <c r="F25" s="11" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="J25" s="2">
         <v>2023</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>83</v>
@@ -8969,7 +9008,7 @@
         <v>26</v>
       </c>
       <c r="O25" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="P25" s="2" t="s">
         <v>26</v>
@@ -9246,29 +9285,29 @@
         <v>26</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="2" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>46</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="J26" s="2">
         <v>2021</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="M26" s="2" t="s">
         <v>83</v>
@@ -9277,7 +9316,7 @@
         <v>26</v>
       </c>
       <c r="O26" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="P26" s="2" t="s">
         <v>26</v>
@@ -9554,29 +9593,29 @@
         <v>26</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="11" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>46</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="J27" s="2">
         <v>2023</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>83</v>
@@ -9585,7 +9624,7 @@
         <v>26</v>
       </c>
       <c r="O27" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="P27" s="2" t="s">
         <v>26</v>
@@ -9851,7 +9890,7 @@
       <c r="JM27" s="2"/>
       <c r="JN27" s="2"/>
     </row>
-    <row r="28" ht="31" hidden="1" spans="1:274">
+    <row r="28" ht="31" spans="1:274">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -9862,35 +9901,35 @@
         <v>26</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="11" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="J28" s="2">
         <v>2024</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>83</v>
       </c>
       <c r="N28" s="6" t="s">
-        <v>26</v>
+        <v>117</v>
       </c>
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
@@ -10162,29 +10201,29 @@
         <v>26</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="2" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>46</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="J29" s="2">
         <v>2024</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="M29" s="2" t="s">
         <v>50</v>
@@ -10198,8 +10237,8 @@
       <c r="P29" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Q29" s="14" t="s">
-        <v>221</v>
+      <c r="Q29" s="4" t="s">
+        <v>230</v>
       </c>
       <c r="R29" s="2"/>
       <c r="S29" s="2"/>
@@ -10459,7 +10498,7 @@
       <c r="JM29" s="2"/>
       <c r="JN29" s="2"/>
     </row>
-    <row r="30" ht="15.5" hidden="1" spans="1:274">
+    <row r="30" ht="15.5" spans="1:274">
       <c r="A30" s="2">
         <v>28</v>
       </c>
@@ -10737,21 +10776,21 @@
       <c r="JM30" s="2"/>
       <c r="JN30" s="2"/>
     </row>
-    <row r="31" ht="31" hidden="1" spans="1:274">
+    <row r="31" ht="31" spans="1:274">
       <c r="A31" s="2">
         <v>29</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="3" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="2"/>
       <c r="G31" s="5" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -10759,7 +10798,7 @@
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
@@ -11023,7 +11062,7 @@
       <c r="JM31" s="2"/>
       <c r="JN31" s="2"/>
     </row>
-    <row r="32" ht="15.5" hidden="1" spans="1:274">
+    <row r="32" ht="15.5" spans="1:274">
       <c r="A32" s="2">
         <v>30</v>
       </c>
@@ -11301,31 +11340,31 @@
       <c r="JM32" s="2"/>
       <c r="JN32" s="2"/>
     </row>
-    <row r="33" ht="31" hidden="1" spans="1:274">
+    <row r="33" ht="31" spans="1:274">
       <c r="A33" s="2">
         <v>31</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="4" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="2" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="J33" s="2">
         <v>2024</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="L33" s="2"/>
       <c r="M33" s="2" t="s">
@@ -11600,37 +11639,37 @@
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="4" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="2" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="J34" s="2">
         <v>2024</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="L34" s="2"/>
       <c r="M34" s="2" t="s">
         <v>25</v>
       </c>
       <c r="N34" s="6" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="O34" s="6" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="P34" s="13" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
@@ -11891,31 +11930,31 @@
       <c r="JM34" s="2"/>
       <c r="JN34" s="2"/>
     </row>
-    <row r="35" ht="31" hidden="1" spans="1:274">
+    <row r="35" ht="31" spans="1:274">
       <c r="A35" s="2">
         <v>33</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="4" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="11" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="J35" s="2">
         <v>2016</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="L35" s="2"/>
       <c r="M35" s="2" t="s">
@@ -12192,14 +12231,14 @@
         <v>26</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="2" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
@@ -12217,7 +12256,7 @@
       </c>
       <c r="P36" s="2"/>
       <c r="Q36" s="4" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="R36" s="2"/>
       <c r="S36" s="2"/>
@@ -12477,7 +12516,7 @@
       <c r="JM36" s="2"/>
       <c r="JN36" s="2"/>
     </row>
-    <row r="37" ht="31" hidden="1" spans="1:274">
+    <row r="37" ht="31" spans="1:274">
       <c r="A37" s="2">
         <v>35</v>
       </c>
@@ -12486,14 +12525,14 @@
         <v>26</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="2" t="s">
-        <v>243</v>
+        <v>252</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
@@ -12504,7 +12543,7 @@
         <v>83</v>
       </c>
       <c r="N37" s="6" t="s">
-        <v>26</v>
+        <v>117</v>
       </c>
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
@@ -12767,14 +12806,14 @@
       <c r="JM37" s="2"/>
       <c r="JN37" s="2"/>
     </row>
-    <row r="38" ht="15.5" hidden="1" spans="1:274">
+    <row r="38" ht="15.5" spans="1:274">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="F38" s="2" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
@@ -14992,13 +15031,6 @@
     </row>
   </sheetData>
   <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:R38" etc:filterBottomFollowUsedRange="0">
-    <filterColumn colId="14">
-      <filters>
-        <filter val="△"/>
-        <filter val="√"/>
-        <filter val="ok"/>
-      </filters>
-    </filterColumn>
     <extLst/>
   </autoFilter>
   <hyperlinks>
@@ -15044,7 +15076,7 @@
     <hyperlink ref="H23" r:id="rId37" display="https://doi.org/10.26180/20011142"/>
     <hyperlink ref="H24" r:id="rId38" display="https://osf.io/35wp9"/>
     <hyperlink ref="H25" r:id="rId39" display="https://osf.io/hbrus/?view_only=98b2095f72e64fd382fc0d33de3f4497"/>
-    <hyperlink ref="H28" r:id="rId40" display="https://osf.io/tsvxy/?view_only=4314d303addf4dff9f443bea774a465a"/>
+    <hyperlink ref="H28" r:id="rId40" display="https://osf.io/tsvxy/?view_only=4314d303addf4dff9f443bea774a465a" tooltip="https://osf.io/tsvxy/?view_only=4314d303addf4dff9f443bea774a465a"/>
     <hyperlink ref="G5" r:id="rId41" display="i.r.kolvoort@uva.nl" tooltip="mailto:i.r.kolvoort@uva.nl"/>
     <hyperlink ref="G14" r:id="rId42" display="s.svensson.19@abdn.ac.uk"/>
     <hyperlink ref="G18" r:id="rId43" display="pastoetter@uni-trier.de" tooltip="mailto:pastoetter@uni-trier.de"/>
@@ -15086,29 +15118,29 @@
         <v>26</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="E1" s="4"/>
       <c r="F1" s="2" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>46</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="J1" s="2">
         <v>2021</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>83</v>
@@ -15117,7 +15149,7 @@
         <v>26</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Update Raw_Data and Clean_Data
</commit_message>
<xml_diff>
--- a/Contact information.xlsx
+++ b/Contact information.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="280">
   <si>
     <t>ID</t>
   </si>
@@ -319,30 +319,6 @@
 Mayan Navon</t>
   </si>
   <si>
-    <t>Does Self-Associating a Geometric Shape Immediately Cause Attentional Prioritization?</t>
-  </si>
-  <si>
-    <t>Gabriela Orellana-Corrales, Christina Matschke, Ann-Katrin Wesslein</t>
-  </si>
-  <si>
-    <t>Gabriela Orellana-Corrales</t>
-  </si>
-  <si>
-    <t>gabyorellanac@gmail.com</t>
-  </si>
-  <si>
-    <t>https://osf.io/3ke4f/</t>
-  </si>
-  <si>
-    <t>G Orellana-Corrales et al.</t>
-  </si>
-  <si>
-    <t>Experimental Psychology</t>
-  </si>
-  <si>
-    <t>Orellana-Corrales_2021_EP</t>
-  </si>
-  <si>
     <t>More or less of me and you: self-relevance augments the effects of item probability on stimulus prioritization</t>
   </si>
   <si>
@@ -568,6 +544,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF212121"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>Dalmaso, M., Vicovaro, M., Sarodo, A., &amp; Watanabe, K. (2024). The self can be associated with novel faces of in-group and out-group members: A cross-cultural study. </t>
     </r>
     <r>
@@ -776,6 +758,9 @@
     <t>Electrophysiological correlates of self‑related processing in adults with autism</t>
   </si>
   <si>
+    <t>Letizia Amodeo,Judith Goris,Annabel D. Nijhof,Jan R. Wiersema</t>
+  </si>
+  <si>
     <t>Letizia Amodeo</t>
   </si>
   <si>
@@ -839,9 +824,6 @@
     <t>Bukowski_2021_AP</t>
   </si>
   <si>
-    <t>TO DO</t>
-  </si>
-  <si>
     <t>Examining the dorsolateral and ventromedial prefrontal cortex involvement in the self-attention network: A randomized, sham-controlled, parallel group, double-blind, and multichannel HD-tDCS study.</t>
   </si>
   <si>
@@ -860,7 +842,7 @@
     <t>Frontiersin</t>
   </si>
   <si>
-    <t>Prof Lucía B. Palmero
+    <t>Lucía B. Palmero
 Víctor Martínez-Pérez</t>
   </si>
   <si>
@@ -915,18 +897,18 @@
     <t>Template_1</t>
   </si>
   <si>
+    <t>Good Me Bad Me: Prioritization of the Good-Self During Perceptual Decision-Making</t>
+  </si>
+  <si>
+    <t>https://osf.io/4zvkm/</t>
+  </si>
+  <si>
+    <t>Collabra: Psychology</t>
+  </si>
+  <si>
     <t>○</t>
   </si>
   <si>
-    <t>Good Me Bad Me: Prioritization of the Good-Self During Perceptual Decision-Making</t>
-  </si>
-  <si>
-    <t>https://osf.io/4zvkm/</t>
-  </si>
-  <si>
-    <t>Collabra: Psychology</t>
-  </si>
-  <si>
     <t>Relevant for Us? We-Prioritization in Cognitive Processing</t>
   </si>
   <si>
@@ -969,6 +951,9 @@
     <t>Schäfer et al.</t>
   </si>
   <si>
+    <t>Experimental Psychology</t>
+  </si>
+  <si>
     <t>Saliency at first sight: instant identity referential advantage toward a newly met partner</t>
   </si>
   <si>
@@ -1003,6 +988,27 @@
   </si>
   <si>
     <t>Journal of Experimental Psychology:Human Perception and Performance</t>
+  </si>
+  <si>
+    <t>Does Self-Associating a Geometric Shape Immediately Cause Attentional Prioritization?</t>
+  </si>
+  <si>
+    <t>Gabriela Orellana-Corrales, Christina Matschke, Ann-Katrin Wesslein</t>
+  </si>
+  <si>
+    <t>Gabriela Orellana-Corrales</t>
+  </si>
+  <si>
+    <t>gabyorellanac@gmail.com</t>
+  </si>
+  <si>
+    <t>https://osf.io/3ke4f/</t>
+  </si>
+  <si>
+    <t>G Orellana-Corrales et al.</t>
+  </si>
+  <si>
+    <t>Orellana-Corrales_2021_EP</t>
   </si>
 </sst>
 </file>
@@ -1051,14 +1057,14 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="宋体"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Times New Roman"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1675,7 +1681,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1683,9 +1689,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1709,10 +1712,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1721,16 +1730,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="6" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2060,11 +2063,11 @@
   <dimension ref="A1:JO37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="L14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M31" sqref="M31"/>
+      <selection pane="bottomRight" activeCell="P43" sqref="P43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -2125,10 +2128,10 @@
       <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="N1" s="14" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="2" t="s">
@@ -2155,25 +2158,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>22</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>25</v>
       </c>
       <c r="J2" s="1" t="s">
@@ -2191,16 +2194,18 @@
       <c r="N2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="O2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="P2" s="7" t="s">
         <v>20</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R2" s="1"/>
+      <c r="R2" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
@@ -2464,22 +2469,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="1"/>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>32</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -2500,16 +2505,16 @@
       <c r="N3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="O3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="P3" s="7" t="s">
         <v>20</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="R3" s="5" t="s">
         <v>40</v>
       </c>
       <c r="S3" s="1"/>
@@ -2775,25 +2780,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>42</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="6" t="s">
         <v>44</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -2811,16 +2816,18 @@
       <c r="N4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="O4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="P4" s="8" t="s">
+      <c r="P4" s="7" t="s">
         <v>20</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R4" s="1"/>
+      <c r="R4" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
@@ -3084,25 +3091,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>49</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="15" t="s">
         <v>52</v>
       </c>
       <c r="J5" s="1" t="s">
@@ -3120,16 +3127,16 @@
       <c r="N5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="O5" s="8" t="s">
+      <c r="O5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="P5" s="8" t="s">
+      <c r="P5" s="7" t="s">
         <v>20</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R5" s="6" t="s">
+      <c r="R5" s="5" t="s">
         <v>56</v>
       </c>
       <c r="S5" s="1"/>
@@ -3397,25 +3404,25 @@
       <c r="B6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>59</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="6" t="s">
         <v>62</v>
       </c>
       <c r="J6" s="1" t="s">
@@ -3433,20 +3440,20 @@
       <c r="N6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="O6" s="8" t="s">
+      <c r="O6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="P6" s="8" t="s">
+      <c r="P6" s="7" t="s">
         <v>20</v>
       </c>
       <c r="Q6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R6" s="6" t="s">
+      <c r="R6" s="5" t="s">
         <v>67</v>
       </c>
       <c r="S6" s="1"/>
-      <c r="T6" s="6"/>
+      <c r="T6" s="5"/>
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -3710,25 +3717,25 @@
       <c r="B7" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>70</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="6" t="s">
         <v>73</v>
       </c>
       <c r="J7" s="1" t="s">
@@ -3746,10 +3753,10 @@
       <c r="N7" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="O7" s="8" t="s">
+      <c r="O7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="P7" s="8" t="s">
+      <c r="P7" s="7" t="s">
         <v>20</v>
       </c>
       <c r="Q7" s="1" t="s">
@@ -3759,7 +3766,7 @@
         <v>71</v>
       </c>
       <c r="S7" s="1"/>
-      <c r="T7" s="6" t="s">
+      <c r="T7" s="5" t="s">
         <v>77</v>
       </c>
       <c r="U7" s="1"/>
@@ -4025,25 +4032,25 @@
       <c r="B8" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>80</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="6" t="s">
         <v>83</v>
       </c>
       <c r="J8" s="1" t="s">
@@ -4059,16 +4066,16 @@
       <c r="N8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="O8" s="8" t="s">
+      <c r="O8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="P8" s="8" t="s">
+      <c r="P8" s="7" t="s">
         <v>20</v>
       </c>
       <c r="Q8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R8" s="6" t="s">
+      <c r="R8" s="5" t="s">
         <v>86</v>
       </c>
       <c r="S8" s="1"/>
@@ -4329,37 +4336,37 @@
       <c r="JN8" s="1"/>
       <c r="JO8" s="1"/>
     </row>
-    <row r="9" ht="31" spans="1:275">
+    <row r="9" ht="46.5" spans="1:275">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1"/>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>88</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="6" t="s">
         <v>91</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>92</v>
       </c>
       <c r="K9" s="1">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>93</v>
@@ -4370,7 +4377,7 @@
       <c r="N9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="O9" s="8" t="s">
+      <c r="O9" s="7" t="s">
         <v>30</v>
       </c>
       <c r="P9" s="1"/>
@@ -4634,53 +4641,59 @@
       <c r="JN9" s="1"/>
       <c r="JO9" s="1"/>
     </row>
-    <row r="10" ht="46.5" spans="1:275">
+    <row r="10" ht="31" spans="1:275">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1"/>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>96</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" s="1">
+        <v>2021</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="K10" s="1">
-        <v>2022</v>
-      </c>
-      <c r="L10" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="N10" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="N10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O10" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
+      <c r="O10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="P10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
@@ -4944,53 +4957,53 @@
         <v>10</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="7" t="s">
         <v>104</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>35</v>
+      <c r="I11" s="6" t="s">
+        <v>107</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="K11" s="1">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="O11" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="O11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="P11" s="8" t="s">
-        <v>20</v>
+      <c r="P11" s="7" t="s">
+        <v>112</v>
       </c>
       <c r="Q11" s="1" t="s">
         <v>20</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>105</v>
+        <v>20</v>
       </c>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
@@ -5250,52 +5263,50 @@
       <c r="JN11" s="1"/>
       <c r="JO11" s="1"/>
     </row>
-    <row r="12" ht="31" spans="1:275">
+    <row r="12" ht="15.5" spans="1:275">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1"/>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>112</v>
+      <c r="E12" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>114</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="I12" s="7" t="s">
         <v>115</v>
       </c>
+      <c r="H12" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>117</v>
+      </c>
       <c r="J12" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="K12" s="1">
         <v>2023</v>
       </c>
-      <c r="L12" s="1" t="s">
-        <v>117</v>
-      </c>
+      <c r="L12" s="1"/>
       <c r="M12" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="O12" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="O12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="P12" s="8" t="s">
-        <v>120</v>
+      <c r="P12" s="7" t="s">
+        <v>112</v>
       </c>
       <c r="Q12" s="1" t="s">
         <v>20</v>
@@ -5561,56 +5572,60 @@
       <c r="JN12" s="1"/>
       <c r="JO12" s="1"/>
     </row>
-    <row r="13" ht="15.5" spans="1:275">
+    <row r="13" ht="46.5" spans="1:275">
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="4" t="s">
+      <c r="B13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="G13" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="H13" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="I13" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="I13" s="7" t="s">
+      <c r="J13" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="K13" s="1">
         <v>2023</v>
       </c>
-      <c r="L13" s="1"/>
+      <c r="L13" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="M13" s="1" t="s">
         <v>127</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="O13" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="O13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="P13" s="8" t="s">
-        <v>120</v>
+      <c r="P13" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="Q13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R13" s="1" t="s">
-        <v>20</v>
+      <c r="R13" s="5" t="s">
+        <v>128</v>
       </c>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
@@ -5870,61 +5885,53 @@
       <c r="JN13" s="1"/>
       <c r="JO13" s="1"/>
     </row>
-    <row r="14" ht="46.5" spans="1:275">
+    <row r="14" ht="31" spans="1:275">
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="B14" s="1"/>
+      <c r="C14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="F14" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>129</v>
       </c>
+      <c r="F14" s="5" t="s">
+        <v>130</v>
+      </c>
       <c r="G14" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="H14" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="H14" s="6" t="s">
         <v>132</v>
       </c>
+      <c r="I14" s="15" t="s">
+        <v>133</v>
+      </c>
       <c r="J14" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="K14" s="1">
         <v>2023</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O14" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="P14" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="R14" s="6" t="s">
-        <v>136</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="O14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
@@ -6188,48 +6195,54 @@
         <v>14</v>
       </c>
       <c r="B15" s="1"/>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="7" t="s">
         <v>138</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="H15" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="I15" s="6" t="s">
         <v>141</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>142</v>
       </c>
       <c r="K15" s="1">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="L15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M15" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="O15" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
+      <c r="O15" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="P15" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
@@ -6488,61 +6501,67 @@
       <c r="JN15" s="1"/>
       <c r="JO15" s="1"/>
     </row>
-    <row r="16" ht="31" spans="1:275">
+    <row r="16" ht="69" customHeight="1" spans="1:275">
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="4" t="s">
+      <c r="B16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="G16" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="H16" s="7" t="s">
+      <c r="I16" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="I16" s="7" t="s">
+      <c r="J16" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" s="1">
+        <v>2022</v>
+      </c>
+      <c r="L16" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="K16" s="1">
-        <v>2021</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>151</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O16" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="O16" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="P16" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q16" s="1" t="s">
+      <c r="P16" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="R16" s="1" t="s">
+      <c r="Q16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
+      <c r="R16" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="S16" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="T16" s="16" t="s">
+        <v>154</v>
+      </c>
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
@@ -6799,67 +6818,59 @@
       <c r="JN16" s="1"/>
       <c r="JO16" s="1"/>
     </row>
-    <row r="17" ht="69" customHeight="1" spans="1:275">
+    <row r="17" ht="31" spans="1:275">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="H17" s="7" t="s">
+      <c r="E17" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="I17" s="7" t="s">
+      <c r="F17" s="5" t="s">
         <v>156</v>
       </c>
+      <c r="G17" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>159</v>
+      </c>
       <c r="J17" s="1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="K17" s="1">
         <v>2022</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="N17" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="O17" s="8" t="s">
+      <c r="O17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P17" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="P17" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q17" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="R17" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="S17" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="T17" s="16" t="s">
-        <v>162</v>
-      </c>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
@@ -7123,50 +7134,54 @@
       <c r="B18" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="G18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="I18" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="H18" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>167</v>
-      </c>
       <c r="J18" s="1" t="s">
-        <v>168</v>
+        <v>74</v>
       </c>
       <c r="K18" s="1">
         <v>2022</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>169</v>
+        <v>93</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="O18" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="P18" s="8" t="s">
+      <c r="O18" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
+      <c r="P18" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
@@ -7430,54 +7445,56 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="J19" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="K19" s="1">
+        <v>2023</v>
+      </c>
+      <c r="L19" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="I19" s="7" t="s">
+      <c r="M19" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K19" s="1">
-        <v>2022</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>174</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="O19" s="8" t="s">
+      <c r="O19" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="P19" s="8" t="s">
-        <v>20</v>
+      <c r="P19" s="7" t="s">
+        <v>112</v>
       </c>
       <c r="Q19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R19" s="1"/>
+      <c r="R19" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
@@ -7741,49 +7758,49 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="F20" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" s="8" t="s">
+      <c r="G20" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="H20" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="G20" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="I20" s="7" t="s">
+      <c r="I20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="K20" s="1">
+        <v>2021</v>
+      </c>
+      <c r="L20" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="K20" s="1">
-        <v>2023</v>
-      </c>
-      <c r="L20" s="1" t="s">
+      <c r="M20" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>181</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="O20" s="8" t="s">
+      <c r="O20" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="P20" s="8" t="s">
-        <v>120</v>
+      <c r="P20" s="7" t="s">
+        <v>112</v>
       </c>
       <c r="Q20" s="1" t="s">
         <v>20</v>
@@ -8049,54 +8066,54 @@
       <c r="JN20" s="1"/>
       <c r="JO20" s="1"/>
     </row>
-    <row r="21" ht="31" spans="1:275">
+    <row r="21" ht="15.5" spans="1:275">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C21" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="F21" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="G21" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="H21" s="6" t="s">
         <v>184</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>185</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>35</v>
       </c>
       <c r="J21" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="K21" s="1">
+        <v>2023</v>
+      </c>
+      <c r="L21" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="K21" s="1">
-        <v>2021</v>
-      </c>
-      <c r="L21" s="1" t="s">
+      <c r="M21" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="N21" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="O21" s="8" t="s">
+      <c r="O21" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="P21" s="8" t="s">
-        <v>120</v>
+      <c r="P21" s="7" t="s">
+        <v>112</v>
       </c>
       <c r="Q21" s="1" t="s">
         <v>20</v>
@@ -8362,60 +8379,60 @@
       <c r="JN21" s="1"/>
       <c r="JO21" s="1"/>
     </row>
-    <row r="22" ht="15.5" spans="1:275">
+    <row r="22" ht="46.5" spans="1:275">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C22" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="F22" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="G22" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="H22" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="H22" s="7" t="s">
+      <c r="I22" s="6" t="s">
         <v>192</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>193</v>
       </c>
       <c r="K22" s="1">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="L22" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="M22" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="N22" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="O22" s="8" t="s">
+      <c r="O22" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P22" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="P22" s="8" t="s">
-        <v>120</v>
       </c>
       <c r="Q22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R22" s="1" t="s">
-        <v>20</v>
+      <c r="R22" s="5" t="s">
+        <v>195</v>
       </c>
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
@@ -8675,59 +8692,57 @@
       <c r="JN22" s="1"/>
       <c r="JO22" s="1"/>
     </row>
-    <row r="23" ht="46.5" spans="1:275">
+    <row r="23" ht="62" spans="1:275">
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" s="4" t="s">
+      <c r="B23" s="1"/>
+      <c r="C23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="G23" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="H23" s="7" t="s">
+      <c r="H23" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="I23" s="7" t="s">
+      <c r="I23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J23" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="K23" s="1">
         <v>2024</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="M23" s="1" t="s">
         <v>202</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O23" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="P23" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="O23" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="P23" s="7" t="s">
         <v>20</v>
       </c>
       <c r="Q23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R23" s="17" t="s">
+      <c r="R23" s="5" t="s">
         <v>203</v>
       </c>
       <c r="S23" s="1"/>
@@ -8988,57 +9003,55 @@
       <c r="JN23" s="1"/>
       <c r="JO23" s="1"/>
     </row>
-    <row r="24" ht="62" spans="1:275">
+    <row r="24" ht="15.5" spans="1:275">
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="4" t="s">
+      <c r="B24" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="F24" s="6"/>
+      <c r="F24" s="5" t="s">
+        <v>205</v>
+      </c>
       <c r="G24" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="H24" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="I24" s="1" t="s">
-        <v>35</v>
+      <c r="H24" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="I24" s="15" t="s">
+        <v>208</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="K24" s="1">
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>208</v>
+        <v>27</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O24" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="P24" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q24" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="R24" s="6" t="s">
-        <v>210</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="O24" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
@@ -9297,32 +9310,30 @@
       <c r="JN24" s="1"/>
       <c r="JO24" s="1"/>
     </row>
-    <row r="25" ht="15.5" spans="1:275">
+    <row r="25" ht="31" spans="1:275">
       <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C25" s="4" t="s">
+      <c r="B25" s="1"/>
+      <c r="C25" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="5" t="s">
         <v>212</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="H25" s="7" t="s">
+      <c r="H25" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="I25" s="7" t="s">
+      <c r="I25" s="6" t="s">
         <v>215</v>
       </c>
       <c r="J25" s="1" t="s">
@@ -9340,7 +9351,7 @@
       <c r="N25" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="O25" s="8" t="s">
+      <c r="O25" s="7" t="s">
         <v>30</v>
       </c>
       <c r="P25" s="1"/>
@@ -9604,51 +9615,49 @@
       <c r="JN25" s="1"/>
       <c r="JO25" s="1"/>
     </row>
-    <row r="26" ht="31" spans="1:275">
+    <row r="26" ht="62" spans="1:275">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="1"/>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="3"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="F26" s="5"/>
+      <c r="G26" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="K26" s="1">
+        <v>2020</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O26" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="K26" s="1">
-        <v>2021</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M26" s="1" t="s">
+      <c r="P26" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="N26" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O26" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
@@ -9907,51 +9916,57 @@
       <c r="JN26" s="1"/>
       <c r="JO26" s="1"/>
     </row>
-    <row r="27" ht="62" spans="1:275">
+    <row r="27" ht="31" spans="1:275">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="1"/>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="6" t="s">
+      <c r="D27" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="F27" s="6"/>
+      <c r="F27" s="5" t="s">
+        <v>227</v>
+      </c>
       <c r="G27" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="H27" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="I27" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="I27" s="7" t="s">
-        <v>229</v>
-      </c>
       <c r="J27" s="1" t="s">
-        <v>230</v>
+        <v>74</v>
       </c>
       <c r="K27" s="1">
         <v>2020</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="M27" s="1"/>
+        <v>229</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>230</v>
+      </c>
       <c r="N27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O27" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="P27" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q27" s="1"/>
-      <c r="R27" s="6" t="s">
-        <v>232</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="O27" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="P27" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q27" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="R27" s="1"/>
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
@@ -10210,54 +10225,42 @@
       <c r="JN27" s="1"/>
       <c r="JO27" s="1"/>
     </row>
-    <row r="28" ht="31" spans="1:275">
+    <row r="28" ht="15.5" spans="1:275">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="E28" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>235</v>
-      </c>
+      <c r="F28" s="5"/>
       <c r="G28" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H28" s="7" t="s">
+      <c r="H28" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="I28" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K28" s="1">
-        <v>2020</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="N28" s="1"/>
-      <c r="O28" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="P28" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="Q28" s="18" t="s">
-        <v>233</v>
-      </c>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="O28" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="P28" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
@@ -10517,41 +10520,45 @@
       <c r="JN28" s="1"/>
       <c r="JO28" s="1"/>
     </row>
-    <row r="29" ht="15.5" spans="1:275">
+    <row r="29" ht="31" spans="1:275">
       <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="11" t="s">
+      <c r="B29" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="F29" s="5"/>
+      <c r="G29" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="J29" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="K29" s="1">
+        <v>2021</v>
+      </c>
+      <c r="L29" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="M29" s="1"/>
+      <c r="N29" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="F29" s="6"/>
-      <c r="G29" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="O29" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="P29" s="8" t="s">
-        <v>240</v>
-      </c>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
@@ -10816,44 +10823,42 @@
       <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="5" t="s">
+      <c r="B30" s="1"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="E30" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="F30" s="7"/>
+      <c r="G30" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="I30" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="F30" s="6"/>
-      <c r="G30" s="1" t="s">
+      <c r="J30" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="K30" s="1">
+        <v>2020</v>
+      </c>
+      <c r="L30" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="I30" s="7" t="s">
-        <v>246</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="K30" s="1">
-        <v>2021</v>
-      </c>
-      <c r="L30" s="1" t="s">
-        <v>248</v>
       </c>
       <c r="M30" s="1"/>
       <c r="N30" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="O30" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="P30" s="8" t="s">
-        <v>250</v>
+        <v>111</v>
+      </c>
+      <c r="O30" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="P30" s="7" t="s">
+        <v>245</v>
       </c>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
@@ -11115,46 +11120,48 @@
       <c r="JN30" s="1"/>
       <c r="JO30" s="1"/>
     </row>
-    <row r="31" ht="31" spans="1:275">
+    <row r="31" ht="15.5" spans="1:275">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" s="1"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="5" t="s">
+      <c r="C31" s="3"/>
+      <c r="D31" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E31" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="F31" s="8"/>
+      <c r="E31" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="F31" s="5"/>
       <c r="G31" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H31" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>252</v>
+        <v>23</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>247</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>126</v>
+        <v>45</v>
       </c>
       <c r="K31" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="M31" s="1"/>
+        <v>248</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>249</v>
+      </c>
       <c r="N31" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="O31" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="P31" s="8" t="s">
-        <v>250</v>
+        <v>241</v>
+      </c>
+      <c r="O31" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="P31" s="7" t="s">
+        <v>245</v>
       </c>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
@@ -11416,50 +11423,52 @@
       <c r="JN31" s="1"/>
       <c r="JO31" s="1"/>
     </row>
-    <row r="32" ht="15.5" spans="1:275">
+    <row r="32" ht="31" spans="1:275">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="1"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="5" t="s">
+      <c r="C32" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="E32" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="F32" s="5"/>
+      <c r="G32" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="K32" s="1">
+        <v>2024</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="M32" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="F32" s="6"/>
-      <c r="G32" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H32" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I32" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K32" s="1">
-        <v>2019</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>257</v>
-      </c>
       <c r="N32" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="O32" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="P32" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="Q32" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="O32" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="P32" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q32" s="17" t="s">
+        <v>225</v>
+      </c>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
@@ -11724,47 +11733,43 @@
         <v>32</v>
       </c>
       <c r="B33" s="1"/>
-      <c r="C33" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E33" s="6" t="s">
+      <c r="C33" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="F33" s="5"/>
+      <c r="G33" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="H33" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="F33" s="6"/>
-      <c r="G33" s="1" t="s">
+      <c r="I33" s="10"/>
+      <c r="J33" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="H33" s="7" t="s">
+      <c r="K33" s="1">
+        <v>2023</v>
+      </c>
+      <c r="L33" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="K33" s="1">
-        <v>2024</v>
-      </c>
-      <c r="L33" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="M33" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="N33" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="O33" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="P33" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="Q33" s="18" t="s">
-        <v>233</v>
-      </c>
+      <c r="M33" s="1"/>
+      <c r="N33" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="O33" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="P33" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
@@ -12029,42 +12034,30 @@
         <v>33</v>
       </c>
       <c r="B34" s="1"/>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="F34" s="5"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="10" t="s">
         <v>263</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="F34" s="6"/>
-      <c r="G34" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="H34" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15" t="s">
-        <v>267</v>
-      </c>
-      <c r="K34" s="1">
-        <v>2023</v>
-      </c>
-      <c r="L34" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="M34" s="1"/>
-      <c r="N34" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="O34" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="P34" s="8" t="s">
-        <v>240</v>
-      </c>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
@@ -12330,27 +12323,31 @@
         <v>34</v>
       </c>
       <c r="B35" s="1"/>
-      <c r="C35" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="E35" s="6" t="s">
+      <c r="C35" s="1"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="F35" s="5"/>
+      <c r="G35" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="K35" s="1">
+        <v>2024</v>
+      </c>
+      <c r="L35" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="F35" s="6"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
       <c r="M35" s="1"/>
-      <c r="N35" s="15" t="s">
-        <v>270</v>
+      <c r="N35" s="1" t="s">
+        <v>241</v>
       </c>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
@@ -12620,30 +12617,30 @@
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="F36" s="6"/>
-      <c r="G36" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="H36" s="7" t="s">
-        <v>273</v>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="F36" s="5"/>
+      <c r="G36" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>270</v>
       </c>
       <c r="I36" s="1"/>
       <c r="J36" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="K36" s="1">
-        <v>2024</v>
+        <v>2016</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="M36" s="1"/>
       <c r="N36" s="1" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
@@ -12912,33 +12909,45 @@
         <v>36</v>
       </c>
       <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6" t="s">
+      <c r="C37" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="H37" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="F37" s="6"/>
-      <c r="G37" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="H37" s="7" t="s">
+      <c r="I37" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="I37" s="1"/>
       <c r="J37" s="1" t="s">
         <v>278</v>
       </c>
       <c r="K37" s="1">
-        <v>2016</v>
+        <v>2020</v>
       </c>
       <c r="L37" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="M37" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="M37" s="1"/>
       <c r="N37" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="O37" s="1"/>
+        <v>241</v>
+      </c>
+      <c r="O37" s="7" t="s">
+        <v>245</v>
+      </c>
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
@@ -13205,64 +13214,64 @@
     <extLst/>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="L24" r:id="rId1" display="Cognitive, Affective, &amp; Behavioral Neuroscience" tooltip="https://link.springer.com/journal/13415"/>
-    <hyperlink ref="H32" r:id="rId2" display="merryndconstable@gmail.com"/>
+    <hyperlink ref="L23" r:id="rId1" display="Cognitive, Affective, &amp; Behavioral Neuroscience" tooltip="https://link.springer.com/journal/13415"/>
+    <hyperlink ref="H31" r:id="rId2" display="merryndconstable@gmail.com"/>
     <hyperlink ref="H2" r:id="rId2" display="merryndconstable@gmail.com" tooltip="mailto:merryndconstable@gmail.com"/>
-    <hyperlink ref="H31" r:id="rId3" display="hcp4715@gmail.com"/>
+    <hyperlink ref="H30" r:id="rId3" display="hcp4715@gmail.com"/>
     <hyperlink ref="H4" r:id="rId2" display="merryndconstable@gmail.com" tooltip="mailto:merryndconstable@gmail.com"/>
     <hyperlink ref="H5" r:id="rId4" display="gaoxp@shnu.edu.cn" tooltip="mailto:gaoxp@shnu.edu.cn"/>
     <hyperlink ref="H6" r:id="rId5" display="schaefer@psychologie-forum-muenster.de" tooltip="mailto:schaefer@psychologie-forum-muenster.de"/>
     <hyperlink ref="H7" r:id="rId6" display="mgwozniak@gmail.com" tooltip="mailto:mgwozniak@gmail.com"/>
-    <hyperlink ref="H30" r:id="rId7" display="skumar@brookes.ac.uk"/>
-    <hyperlink ref="H25" r:id="rId8" display="marius.golubickis@abdn.ac.uk" tooltip="mailto:marius.golubickis@abdn.ac.uk"/>
+    <hyperlink ref="H29" r:id="rId7" display="skumar@brookes.ac.uk"/>
+    <hyperlink ref="H24" r:id="rId8" display="marius.golubickis@abdn.ac.uk" tooltip="mailto:marius.golubickis@abdn.ac.uk"/>
     <hyperlink ref="H8" r:id="rId9" display="mayanna@post.bgu.ac.il" tooltip="mailto:mayanna@post.bgu.ac.il"/>
-    <hyperlink ref="H9" r:id="rId10" display="gabyorellanac@gmail.com" tooltip="mailto:gabyorellanac@gmail.com"/>
-    <hyperlink ref="H13" r:id="rId3" display="hcp4715@gmail.com"/>
-    <hyperlink ref="H20" r:id="rId11" display="wf3126@mail.tsinghua.edu.cn" tooltip="mailto:wf3126@mail.tsinghua.edu.cn"/>
-    <hyperlink ref="H22" r:id="rId12" display="jie.sui@abdn.ac.uk"/>
-    <hyperlink ref="H23" r:id="rId13" display="lfuentes@um.es" tooltip="mailto:lfuentes@um.es"/>
-    <hyperlink ref="H35" r:id="rId14" display="tseng@riec.tohoku.ac.jp"/>
-    <hyperlink ref="H34" r:id="rId15" display="wentura@mx.uni-saarland.de" tooltip="mailto:wentura@mx.uni-saarland.de"/>
-    <hyperlink ref="H36" r:id="rId16" display="marcel.pauly@uni-saarlande.de"/>
-    <hyperlink ref="H33" r:id="rId17" display="mario.dalmaso@unipd.it"/>
-    <hyperlink ref="H37" r:id="rId18" display="jie.sui@psy.ox.ac.uk"/>
-    <hyperlink ref="I32" r:id="rId19" display="https://osf.io/sejw7/"/>
+    <hyperlink ref="H37" r:id="rId10" display="gabyorellanac@gmail.com" tooltip="mailto:gabyorellanac@gmail.com"/>
+    <hyperlink ref="H12" r:id="rId3" display="hcp4715@gmail.com"/>
+    <hyperlink ref="H19" r:id="rId11" display="wf3126@mail.tsinghua.edu.cn" tooltip="mailto:wf3126@mail.tsinghua.edu.cn"/>
+    <hyperlink ref="H21" r:id="rId12" display="jie.sui@abdn.ac.uk"/>
+    <hyperlink ref="H22" r:id="rId13" display="lfuentes@um.es" tooltip="mailto:lfuentes@um.es"/>
+    <hyperlink ref="H34" r:id="rId14" display="tseng@riec.tohoku.ac.jp"/>
+    <hyperlink ref="H33" r:id="rId15" display="wentura@mx.uni-saarland.de" tooltip="mailto:wentura@mx.uni-saarland.de"/>
+    <hyperlink ref="H35" r:id="rId16" display="marcel.pauly@uni-saarlande.de"/>
+    <hyperlink ref="H32" r:id="rId17" display="mario.dalmaso@unipd.it"/>
+    <hyperlink ref="H36" r:id="rId18" display="jie.sui@psy.ox.ac.uk"/>
+    <hyperlink ref="I31" r:id="rId19" display="https://osf.io/sejw7/"/>
     <hyperlink ref="I2" r:id="rId20" display="https://osf.io/5zaej/"/>
-    <hyperlink ref="I31" r:id="rId21" display="https://osf.io/4zvkm/"/>
-    <hyperlink ref="I30" r:id="rId22" display="https://figshare.com/s/e1391ebe3f11e8d70d9f" tooltip="https://figshare.com/s/e1391ebe3f11e8d70d9f"/>
+    <hyperlink ref="I30" r:id="rId21" display="https://osf.io/4zvkm/"/>
+    <hyperlink ref="I29" r:id="rId22" display="https://figshare.com/s/e1391ebe3f11e8d70d9f" tooltip="https://figshare.com/s/e1391ebe3f11e8d70d9f"/>
     <hyperlink ref="I4" r:id="rId23" display="https://osf.io/khyjq/"/>
     <hyperlink ref="I5" r:id="rId24" display="https://osf.io/bw27c"/>
     <hyperlink ref="I6" r:id="rId25" display="http://dx.doi.org/10.23668/psycharchives.2642"/>
     <hyperlink ref="I7" r:id="rId26" display="https://journals.plos.org/plosone/article?id=10.1371/journal.pone.0190679#sec025"/>
-    <hyperlink ref="I25" r:id="rId27" display="https://osf.io/8bktn/" tooltip="https://osf.io/8bktn/"/>
+    <hyperlink ref="I24" r:id="rId27" display="https://osf.io/8bktn/" tooltip="https://osf.io/8bktn/"/>
     <hyperlink ref="I8" r:id="rId28" display="https://osf.io/4srhn/?view_only=70ea4888bf524b598b0d61d04a54d9d9"/>
-    <hyperlink ref="I9" r:id="rId29" display="https://osf.io/3ke4f/"/>
-    <hyperlink ref="I10" r:id="rId30" display="https://osf.io/cj7fp/"/>
-    <hyperlink ref="I12" r:id="rId31" display="https://osf.io/4n6j7/"/>
-    <hyperlink ref="I13" r:id="rId32" display="https://zenodo.org/records/8031086"/>
-    <hyperlink ref="I14" r:id="rId33" display="https://osf.io/2juxk/?view_only=b4e01124337a4801b4beb99dbe803b8d"/>
-    <hyperlink ref="I15" r:id="rId34" display="https://researchdata.bath.ac.uk/924/" tooltip="https://researchdata.bath.ac.uk/924/"/>
-    <hyperlink ref="I16" r:id="rId35" display="https://osf.io/u9ty6/?view_only=9bdbbaf95f9a4d9c8bc53dd1a29563ae."/>
-    <hyperlink ref="I17" r:id="rId36" display="https://doi.org/10.17605/OSF.IO/FE3JW"/>
-    <hyperlink ref="I18" r:id="rId37" display="https://doi.org/10.26180/20011142"/>
-    <hyperlink ref="I19" r:id="rId38" display="https://osf.io/35wp9"/>
-    <hyperlink ref="I20" r:id="rId39" display="https://osf.io/hbrus/?view_only=98b2095f72e64fd382fc0d33de3f4497"/>
-    <hyperlink ref="I23" r:id="rId40" display="https://osf.io/tsvxy/?view_only=4314d303addf4dff9f443bea774a465a" tooltip="https://osf.io/tsvxy/?view_only=4314d303addf4dff9f443bea774a465a"/>
+    <hyperlink ref="I37" r:id="rId29" display="https://osf.io/3ke4f/" tooltip="https://osf.io/3ke4f/"/>
+    <hyperlink ref="I9" r:id="rId30" display="https://osf.io/cj7fp/"/>
+    <hyperlink ref="I11" r:id="rId31" display="https://osf.io/4n6j7/"/>
+    <hyperlink ref="I12" r:id="rId32" display="https://zenodo.org/records/8031086"/>
+    <hyperlink ref="I13" r:id="rId33" display="https://osf.io/2juxk/?view_only=b4e01124337a4801b4beb99dbe803b8d"/>
+    <hyperlink ref="I14" r:id="rId34" display="https://researchdata.bath.ac.uk/924/" tooltip="https://researchdata.bath.ac.uk/924/"/>
+    <hyperlink ref="I15" r:id="rId35" display="https://osf.io/u9ty6/?view_only=9bdbbaf95f9a4d9c8bc53dd1a29563ae."/>
+    <hyperlink ref="I16" r:id="rId36" display="https://doi.org/10.17605/OSF.IO/FE3JW"/>
+    <hyperlink ref="I17" r:id="rId37" display="https://doi.org/10.26180/20011142"/>
+    <hyperlink ref="I18" r:id="rId38" display="https://osf.io/35wp9"/>
+    <hyperlink ref="I19" r:id="rId39" display="https://osf.io/hbrus/?view_only=98b2095f72e64fd382fc0d33de3f4497"/>
+    <hyperlink ref="I22" r:id="rId40" display="https://osf.io/tsvxy/?view_only=4314d303addf4dff9f443bea774a465a" tooltip="https://osf.io/tsvxy/?view_only=4314d303addf4dff9f443bea774a465a"/>
     <hyperlink ref="H3" r:id="rId41" display="i.r.kolvoort@uva.nl" tooltip="mailto:i.r.kolvoort@uva.nl"/>
-    <hyperlink ref="H10" r:id="rId42" display="s.svensson.19@abdn.ac.uk"/>
-    <hyperlink ref="H14" r:id="rId43" display="pastoetter@uni-trier.de" tooltip="mailto:pastoetter@uni-trier.de"/>
-    <hyperlink ref="H15" r:id="rId44" display="c.hobbs@bristol.ac.uk;" tooltip="mailto:c.hobbs@bristol.ac.uk;"/>
-    <hyperlink ref="H17" r:id="rId45" display="michele.vicovaro@unipd.it"/>
-    <hyperlink ref="H18" r:id="rId46" display="kelsey.perrykkad@monash.edu"/>
-    <hyperlink ref="H19" r:id="rId6" display="mgwozniak@gmail.com" tooltip="mailto:mgwozniak@gmail.com"/>
-    <hyperlink ref="H24" r:id="rId47" display="letizia.amodeo@ugent.be"/>
-    <hyperlink ref="H27" r:id="rId48" display="victor.martinez5@um.es" tooltip="mailto:victor.martinez5@um.es"/>
-    <hyperlink ref="H26" r:id="rId49" display="hbbukowski@gmail.com"/>
-    <hyperlink ref="H21" r:id="rId50" display="hongjl18@mails.tsinghua.edu.cn" tooltip="mailto:hongjl18@mails.tsinghua.edu.cn"/>
-    <hyperlink ref="H11" r:id="rId51" display="guanll353@nenu.edu.cn"/>
-    <hyperlink ref="I28" r:id="rId52" display="https://osf.io/2q9w7/" tooltip="https://osf.io/2q9w7/"/>
-    <hyperlink ref="I27" r:id="rId53" display="https://www.frontiersin.org/journals/neuroscience/articles/10.3389/fnins.2020.00683/full" tooltip="https://www.frontiersin.org/journals/neuroscience/articles/10.3389/fnins.2020.00683/full"/>
-    <hyperlink ref="I26" r:id="rId54" display="https://osf.io/pcv3u/"/>
+    <hyperlink ref="H9" r:id="rId42" display="s.svensson.19@abdn.ac.uk"/>
+    <hyperlink ref="H13" r:id="rId43" display="pastoetter@uni-trier.de" tooltip="mailto:pastoetter@uni-trier.de"/>
+    <hyperlink ref="H14" r:id="rId44" display="c.hobbs@bristol.ac.uk;" tooltip="mailto:c.hobbs@bristol.ac.uk;"/>
+    <hyperlink ref="H16" r:id="rId45" display="michele.vicovaro@unipd.it"/>
+    <hyperlink ref="H17" r:id="rId46" display="kelsey.perrykkad@monash.edu"/>
+    <hyperlink ref="H18" r:id="rId6" display="mgwozniak@gmail.com" tooltip="mailto:mgwozniak@gmail.com"/>
+    <hyperlink ref="H23" r:id="rId47" display="letizia.amodeo@ugent.be"/>
+    <hyperlink ref="H26" r:id="rId48" display="victor.martinez5@um.es" tooltip="mailto:victor.martinez5@um.es"/>
+    <hyperlink ref="H25" r:id="rId49" display="hbbukowski@gmail.com"/>
+    <hyperlink ref="H20" r:id="rId50" display="hongjl18@mails.tsinghua.edu.cn" tooltip="mailto:hongjl18@mails.tsinghua.edu.cn"/>
+    <hyperlink ref="H10" r:id="rId51" display="guanll353@nenu.edu.cn"/>
+    <hyperlink ref="I27" r:id="rId52" display="https://osf.io/2q9w7/" tooltip="https://osf.io/2q9w7/"/>
+    <hyperlink ref="I26" r:id="rId53" display="https://www.frontiersin.org/journals/neuroscience/articles/10.3389/fnins.2020.00683/full" tooltip="https://www.frontiersin.org/journals/neuroscience/articles/10.3389/fnins.2020.00683/full"/>
+    <hyperlink ref="I25" r:id="rId54" display="https://osf.io/pcv3u/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Update Remove 1 Paper
Bukowski_2021_AP
</commit_message>
<xml_diff>
--- a/Contact information.xlsx
+++ b/Contact information.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Label!$A$1:$S$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Label!$A$1:$S$39</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="283">
   <si>
     <t>ID</t>
   </si>
@@ -96,141 +96,61 @@
     <t>√</t>
   </si>
   <si>
-    <t>Sticking together? Re-binding previous other-associated stimuli interferes with self-verification but not partner-verification</t>
-  </si>
-  <si>
-    <t>Merryn D. Constable, Fruzsina Elekes, Natalie Sebanz, and Günther Knoblich</t>
-  </si>
-  <si>
-    <t>Merryn D. Constable</t>
-  </si>
-  <si>
-    <t>merryndconstable@gmail.com</t>
-  </si>
-  <si>
-    <t>https://osf.io/5zaej/</t>
-  </si>
-  <si>
-    <t>Constable &amp; Knoblich</t>
+    <t>Electrophysiological correlates of self‑related processing in adults with autism</t>
+  </si>
+  <si>
+    <t>Letizia Amodeo,Judith Goris,Annabel D. Nijhof,Jan R. Wiersema</t>
+  </si>
+  <si>
+    <t>Letizia Amodeo</t>
+  </si>
+  <si>
+    <t>letizia.amodeo@ugent.be</t>
+  </si>
+  <si>
+    <t>Can be obtained via request</t>
+  </si>
+  <si>
+    <t>L Amodeo et al.</t>
+  </si>
+  <si>
+    <t>Cognitive, Affective, &amp; Behavioral Neuroscience</t>
+  </si>
+  <si>
+    <t>Amodeo_2024_CABN</t>
+  </si>
+  <si>
+    <t>Template_2</t>
+  </si>
+  <si>
+    <t>Letizia Amodeo
+Judith Goris
+Annabel D. Nijhof
+Jan R. Wiersema</t>
+  </si>
+  <si>
+    <t>Socio-cognitive training impacts emotional and perceptual self-salience but not self-other distinction.</t>
+  </si>
+  <si>
+    <t>Henryk Bukowski,Boryana Todorova,Magdalena Boch,Giorgia Silani,Claus Lamm</t>
+  </si>
+  <si>
+    <t>Henryk Bukowski</t>
+  </si>
+  <si>
+    <t>hbbukowski@gmail.com</t>
+  </si>
+  <si>
+    <t>https://osf.io/pcv3u/</t>
+  </si>
+  <si>
+    <t>Henryk Bukowski et al.</t>
   </si>
   <si>
     <t>Acta Psychologica</t>
   </si>
   <si>
-    <t>Constable_2020_AP</t>
-  </si>
-  <si>
-    <t>Template_2+询问P1、P2对应的Identity</t>
-  </si>
-  <si>
-    <t>√√</t>
-  </si>
-  <si>
-    <t>Temporal integration as “common currency” of brain and self-scale-free activity in resting-state EEG correlates with temporal delay effects on self-relatedness</t>
-  </si>
-  <si>
-    <t>Ivar R. Kolvoort,Soren Wainio-Theberge,Annemarie Wolff,Georg Northoff</t>
-  </si>
-  <si>
-    <t>Ivar R. Kolvoort</t>
-  </si>
-  <si>
-    <t>i.r.kolvoort@uva.nl</t>
-  </si>
-  <si>
-    <t>Can be obtained via request</t>
-  </si>
-  <si>
-    <t>IR Kolvoort et al.</t>
-  </si>
-  <si>
-    <t>Human Brain Mapping</t>
-  </si>
-  <si>
-    <t>Kolvoort_2020_HBM</t>
-  </si>
-  <si>
-    <t>Template_2</t>
-  </si>
-  <si>
-    <t>Ivar Kolvoort
-Georg Northoff</t>
-  </si>
-  <si>
-    <t>Affective compatibility with the self modulates the self-prioritisation effect</t>
-  </si>
-  <si>
-    <t>Merryn Dale Constable , Maike Lena Becker , Ye-In Oh &amp; Günther Knoblich</t>
-  </si>
-  <si>
-    <t>Merryn Dale Constable</t>
-  </si>
-  <si>
-    <t>https://osf.io/khyjq/</t>
-  </si>
-  <si>
-    <t>Constable et al.</t>
-  </si>
-  <si>
-    <t>Cognition and Emotion</t>
-  </si>
-  <si>
-    <t>Constable_2020_CE</t>
-  </si>
-  <si>
-    <t>Prioritised self-referential processing is modulated by emotional arousal</t>
-  </si>
-  <si>
-    <t>Haoyue Qian, Zhiguo Wang, Chao Li, Xiangping Gao</t>
-  </si>
-  <si>
-    <t>Xiangping Gao</t>
-  </si>
-  <si>
-    <t>gaoxp@shnu.edu.cn</t>
-  </si>
-  <si>
-    <t>https://osf.io/bw27c</t>
-  </si>
-  <si>
-    <t>Qian et al.</t>
-  </si>
-  <si>
-    <t>Quarterly Journal of Experimental Psychology</t>
-  </si>
-  <si>
-    <t>Qian_2019_QJEP</t>
-  </si>
-  <si>
-    <t>Xiangping Gao
-Haoyue Qian</t>
-  </si>
-  <si>
-    <t>CC-BY-SA 4.0</t>
-  </si>
-  <si>
-    <t>Understanding self-prioritisation: the prioritisation of self-relevant stimuli and its relation to the individual self-esteem</t>
-  </si>
-  <si>
-    <t>Sarah Schäfer and Christian Frings</t>
-  </si>
-  <si>
-    <t>Sarah Schäfer</t>
-  </si>
-  <si>
-    <t>schaefer@psychologie-forum-muenster.de</t>
-  </si>
-  <si>
-    <t>http://dx.doi.org/10.23668/psycharchives.2642</t>
-  </si>
-  <si>
-    <t>Schäfer &amp; Frings</t>
-  </si>
-  <si>
-    <t>Journal of Cognitive Psychology</t>
-  </si>
-  <si>
-    <t>Schaefer_2019_CP</t>
+    <t>Bukowski_2021_AP</t>
   </si>
   <si>
     <r>
@@ -253,36 +173,91 @@
     </r>
   </si>
   <si>
-    <t>Sarah Schäfer
-Marel Pauly
-Dirk Wentura</t>
-  </si>
-  <si>
-    <t>CC BY 4.0</t>
-  </si>
-  <si>
-    <t>Prioritization of arbitrary faces associated to self: An EEG study</t>
-  </si>
-  <si>
-    <t>Mateusz Woźniak, Dimitrios Kourtis, Gunther Knoblich</t>
-  </si>
-  <si>
-    <t>Mateusz Wozniak</t>
-  </si>
-  <si>
-    <t>mgwozniak@gmail.com</t>
-  </si>
-  <si>
-    <t>https://journals.plos.org/plosone/article?id=10.1371/journal.pone.0190679#sec025</t>
-  </si>
-  <si>
-    <t>Woźniak et al.</t>
-  </si>
-  <si>
-    <t>PloS one</t>
-  </si>
-  <si>
-    <t>Wozniak_2018_PLOS</t>
+    <t>√√</t>
+  </si>
+  <si>
+    <t>Relevant for Us? We-Prioritization in Cognitive Processing</t>
+  </si>
+  <si>
+    <t>Merryn D. Constable</t>
+  </si>
+  <si>
+    <t>merryndconstable@gmail.com</t>
+  </si>
+  <si>
+    <t>https://osf.io/sejw7/</t>
+  </si>
+  <si>
+    <t>Constable et al.</t>
+  </si>
+  <si>
+    <t>Journal of Experimental Psychology:  Human Perception and Performance</t>
+  </si>
+  <si>
+    <t>Constable_2019_EPHPP</t>
+  </si>
+  <si>
+    <t>Template_1</t>
+  </si>
+  <si>
+    <t>○</t>
+  </si>
+  <si>
+    <t>Sticking together? Re-binding previous other-associated stimuli interferes with self-verification but not partner-verification</t>
+  </si>
+  <si>
+    <t>Merryn D. Constable, Fruzsina Elekes, Natalie Sebanz, and Günther Knoblich</t>
+  </si>
+  <si>
+    <t>https://osf.io/5zaej/</t>
+  </si>
+  <si>
+    <t>Constable &amp; Knoblich</t>
+  </si>
+  <si>
+    <t>Constable_2020_AP</t>
+  </si>
+  <si>
+    <t>Template_2+询问P1、P2对应的Identity</t>
+  </si>
+  <si>
+    <t>Affective compatibility with the self modulates the self-prioritisation effect</t>
+  </si>
+  <si>
+    <t>Merryn Dale Constable , Maike Lena Becker , Ye-In Oh &amp; Günther Knoblich</t>
+  </si>
+  <si>
+    <t>Merryn Dale Constable</t>
+  </si>
+  <si>
+    <t>https://osf.io/khyjq/</t>
+  </si>
+  <si>
+    <t>Cognition and Emotion</t>
+  </si>
+  <si>
+    <t>Constable_2020_CE</t>
+  </si>
+  <si>
+    <t>△</t>
+  </si>
+  <si>
+    <t>The self can be associated with novel faces of in-group and out-group members: A cross-cultural study</t>
+  </si>
+  <si>
+    <t>Mario Dalmaso</t>
+  </si>
+  <si>
+    <t>mario.dalmaso@unipd.it</t>
+  </si>
+  <si>
+    <t>Mario Dalmaso et al.</t>
+  </si>
+  <si>
+    <t>Consciousness and Cognition</t>
+  </si>
+  <si>
+    <t>Dalmaso_2024_CC</t>
   </si>
   <si>
     <t>2022.https://osf.io/f2bg6/ √
@@ -291,148 +266,55 @@
 2022.https://osf.io/qsr4e/√</t>
   </si>
   <si>
-    <t>CC0 1.0 Universal</t>
-  </si>
-  <si>
-    <t>Are Self-Related Items Unique? The Self-Prioritization Effect Revisited</t>
-  </si>
-  <si>
-    <t>Mayan Navon, Tal Makovski</t>
-  </si>
-  <si>
-    <t>Mayan Navon</t>
-  </si>
-  <si>
-    <t>mayanna@post.bgu.ac.il</t>
-  </si>
-  <si>
-    <t>https://osf.io/4srhn/?view_only=70ea4888bf524b598b0d61d04a54d9d9</t>
-  </si>
-  <si>
-    <t>Navon &amp; Makovski</t>
-  </si>
-  <si>
-    <t>Navon_2021</t>
-  </si>
-  <si>
-    <t>Tal Makovski
-Mayan Navon</t>
-  </si>
-  <si>
-    <t>More or less of me and you: self-relevance augments the effects of item probability on stimulus prioritization</t>
-  </si>
-  <si>
-    <t>Saga L. Svensson, Marius Golubickis, Hollie Maclean, Johanna K. Falbén, Linn M. Persson, Dimitra Tsamadi, Siobhan Caughey, Arash Sahraie, C. Neil Macrae</t>
-  </si>
-  <si>
-    <t>Saga L. Svensson</t>
-  </si>
-  <si>
-    <t>s.svensson.19@abdn.ac.uk</t>
-  </si>
-  <si>
-    <t>https://osf.io/cj7fp/</t>
-  </si>
-  <si>
-    <t>Svensson et al.</t>
-  </si>
-  <si>
-    <t>Psychological Research</t>
-  </si>
-  <si>
-    <t>Svensson_2021_PR</t>
-  </si>
-  <si>
-    <t>Romantic feedbacks influence self-relevant processing: the moderating effects of sex difference and facial attractiveness</t>
-  </si>
-  <si>
-    <t>Yang Xu, Yuan Yuan, Xiaochun Xie, Hui Tan, Lili Guan</t>
-  </si>
-  <si>
-    <t>Lili Guan</t>
-  </si>
-  <si>
-    <t>guanll353@nenu.edu.cn</t>
-  </si>
-  <si>
-    <t>Xu et al.</t>
-  </si>
-  <si>
-    <t>Current Psychology</t>
-  </si>
-  <si>
-    <t>Xu_2021_CP</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Template_2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>（未公开数据）</t>
-    </r>
-  </si>
-  <si>
-    <t>To see or not to see: the parallel processing of self-relevance and facial expressions</t>
-  </si>
-  <si>
-    <t>Tuo Liu, Jie Sui and Andrea Hildebrandt</t>
-  </si>
-  <si>
-    <t>Tuo Liu</t>
-  </si>
-  <si>
-    <t>tuo.liu@uol.de</t>
-  </si>
-  <si>
-    <t>https://osf.io/4n6j7/</t>
-  </si>
-  <si>
-    <t>Liu et al.</t>
-  </si>
-  <si>
-    <t>Cognitive Research: Principles and Implications</t>
-  </si>
-  <si>
-    <t>Liu_2023_CP</t>
-  </si>
-  <si>
-    <t>OK</t>
+    <t>CC BY 4.0</t>
+  </si>
+  <si>
+    <t>Perceiving the Self and Emotions with an Anxious Mind:Evidence from an Implicit Perceptual Task</t>
+  </si>
+  <si>
+    <t>Michella Feldborg,Naomi A. Lee,Kalai Hung,Kaiping Peng,Jie Sui</t>
+  </si>
+  <si>
+    <t>Kalai Hung</t>
+  </si>
+  <si>
+    <t>hongjl18@mails.tsinghua.edu.cn</t>
+  </si>
+  <si>
+    <t>M Feldborg et al.</t>
+  </si>
+  <si>
+    <t>International Journal of Environmental Research and Public Health</t>
+  </si>
+  <si>
+    <t>Feldborg_2021_ERPH</t>
   </si>
   <si>
     <t>ok</t>
   </si>
   <si>
-    <t>Self-referencing prioritizes moral character on perceptual matching</t>
-  </si>
-  <si>
-    <t>Hu Chuan-Peng, Kaiping Peng, Jie Sui</t>
-  </si>
-  <si>
-    <t>Chuan-Peng Hu</t>
-  </si>
-  <si>
-    <t>hcp4715@gmail.com</t>
-  </si>
-  <si>
-    <t>https://zenodo.org/records/8031086</t>
-  </si>
-  <si>
-    <t>Hu et al.</t>
-  </si>
-  <si>
-    <t>Hu_2023</t>
+    <t>CC BY-NC-ND</t>
+  </si>
+  <si>
+    <t>Judging me and you: Task design modulates self-prioritization</t>
+  </si>
+  <si>
+    <t>Marius Golubickis,C. Neil Macrae</t>
+  </si>
+  <si>
+    <t>Marius Golubickis</t>
+  </si>
+  <si>
+    <t>marius.golubickis@abdn.ac.uk</t>
+  </si>
+  <si>
+    <t>https://osf.io/8bktn/</t>
+  </si>
+  <si>
+    <t>Golubickis &amp; Macrae</t>
+  </si>
+  <si>
+    <t>Golubickis_2021_AP</t>
   </si>
   <si>
     <t>The oscillatory fingerprints of self-prioritization: Novel markers in spectral EEG for self-relevant processing</t>
@@ -489,6 +371,55 @@
     <t>Hobbs_2023_PM</t>
   </si>
   <si>
+    <t>Self-referencing prioritizes moral character on perceptual matching</t>
+  </si>
+  <si>
+    <t>Hu Chuan-Peng, Kaiping Peng, Jie Sui</t>
+  </si>
+  <si>
+    <t>Chuan-Peng Hu</t>
+  </si>
+  <si>
+    <t>hcp4715@gmail.com</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/8031086</t>
+  </si>
+  <si>
+    <t>Hu et al.</t>
+  </si>
+  <si>
+    <t>Hu_2023</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Temporal integration as “common currency” of brain and self-scale-free activity in resting-state EEG correlates with temporal delay effects on self-relatedness</t>
+  </si>
+  <si>
+    <t>Ivar R. Kolvoort,Soren Wainio-Theberge,Annemarie Wolff,Georg Northoff</t>
+  </si>
+  <si>
+    <t>Ivar R. Kolvoort</t>
+  </si>
+  <si>
+    <t>i.r.kolvoort@uva.nl</t>
+  </si>
+  <si>
+    <t>IR Kolvoort et al.</t>
+  </si>
+  <si>
+    <t>Human Brain Mapping</t>
+  </si>
+  <si>
+    <t>Kolvoort_2020_HBM</t>
+  </si>
+  <si>
+    <t>Ivar Kolvoort
+Georg Northoff</t>
+  </si>
+  <si>
     <t>The roles of the LpSTS and DLPFC in self-prioritization: A transcranial magnetic stimulation study</t>
   </si>
   <si>
@@ -510,37 +441,54 @@
     <t>Liang_2021_HBM</t>
   </si>
   <si>
-    <t>Towards The Boundaries of Self-Prioritization: Associating The Self With Asymmetric Shapes Disrupts The Self-Prioritization Effect</t>
-  </si>
-  <si>
-    <t>Michele Vicovaro,Mario Dalmaso,Marco Bertamini</t>
-  </si>
-  <si>
-    <t>Michele Vicovaro</t>
-  </si>
-  <si>
-    <t>michele.vicovaro@unipd.it</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.17605/OSF.IO/FE3JW</t>
-  </si>
-  <si>
-    <t>Vicovaro et al.</t>
-  </si>
-  <si>
-    <t>Journal of Experimental Psychology: Human Perception and Performance</t>
-  </si>
-  <si>
-    <t>Vicovaro_2022_EPHPP</t>
-  </si>
-  <si>
-    <t>Mario Dalmaso (Department of Social and Developmental Psychology, University of Padova)
-Marco Bertamini (Department of General Psychology, University of Padova)
-Michele Vicovaro</t>
-  </si>
-  <si>
-    <t>Sarah Schäfer
-Marius Golubickis</t>
+    <t>To see or not to see: the parallel processing of self-relevance and facial expressions</t>
+  </si>
+  <si>
+    <t>Tuo Liu, Jie Sui and Andrea Hildebrandt</t>
+  </si>
+  <si>
+    <t>Tuo Liu</t>
+  </si>
+  <si>
+    <t>tuo.liu@uol.de</t>
+  </si>
+  <si>
+    <t>https://osf.io/4n6j7/</t>
+  </si>
+  <si>
+    <t>Liu et al.</t>
+  </si>
+  <si>
+    <t>Cognitive Research: Principles and Implications</t>
+  </si>
+  <si>
+    <t>Liu_2023_CP</t>
+  </si>
+  <si>
+    <t>Self-prioritization effect in the attentional blink paradigm: Attention-based or familiarity-based effect?</t>
+  </si>
+  <si>
+    <t>Víctor Martínez-Perez,Alejandro Sandoval-Lentisco,Miriam Tortajada,Lucía B. Palmero,Guillermo Campoy,Luis J. Fuentes</t>
+  </si>
+  <si>
+    <t>Luis J. Fuentes</t>
+  </si>
+  <si>
+    <t>lfuentes@um.es</t>
+  </si>
+  <si>
+    <t>https://osf.io/tsvxy/?view_only=4314d303addf4dff9f443bea774a465a</t>
+  </si>
+  <si>
+    <t>V Martínez-Pérez et al.</t>
+  </si>
+  <si>
+    <t>Martinez-Perez_2024_CC</t>
+  </si>
+  <si>
+    <t>Victor Martinez-Perez,
+Lucía B. Palmero,
+Luis J. Fuentes</t>
   </si>
   <si>
     <r>
@@ -630,6 +578,58 @@
     </r>
   </si>
   <si>
+    <t>CC0 1.0 Universal</t>
+  </si>
+  <si>
+    <t>Are Self-Related Items Unique? The Self-Prioritization Effect Revisited</t>
+  </si>
+  <si>
+    <t>Mayan Navon, Tal Makovski</t>
+  </si>
+  <si>
+    <t>Mayan Navon</t>
+  </si>
+  <si>
+    <t>mayanna@post.bgu.ac.il</t>
+  </si>
+  <si>
+    <t>https://osf.io/4srhn/?view_only=70ea4888bf524b598b0d61d04a54d9d9</t>
+  </si>
+  <si>
+    <t>Navon &amp; Makovski</t>
+  </si>
+  <si>
+    <t>Navon_2021</t>
+  </si>
+  <si>
+    <t>Tal Makovski
+Mayan Navon</t>
+  </si>
+  <si>
+    <t>Does Self-Associating a Geometric Shape Immediately Cause Attentional Prioritization?</t>
+  </si>
+  <si>
+    <t>Gabriela Orellana-Corrales, Christina Matschke, Ann-Katrin Wesslein</t>
+  </si>
+  <si>
+    <t>Gabriela Orellana-Corrales</t>
+  </si>
+  <si>
+    <t>gabyorellanac@gmail.com</t>
+  </si>
+  <si>
+    <t>https://osf.io/3ke4f/</t>
+  </si>
+  <si>
+    <t>G Orellana-Corrales et al.</t>
+  </si>
+  <si>
+    <t>Experimental Psychology</t>
+  </si>
+  <si>
+    <t>Orellana-Corrales_2021_EP</t>
+  </si>
+  <si>
     <t>How selves difer within and across cognitive domains: self-prioritisation, self-concept, and psychiatric traits</t>
   </si>
   <si>
@@ -654,6 +654,189 @@
     <t>Perrykkad_2022_BMC</t>
   </si>
   <si>
+    <t>Prioritised self-referential processing is modulated by emotional arousal</t>
+  </si>
+  <si>
+    <t>Haoyue Qian, Zhiguo Wang, Chao Li, Xiangping Gao</t>
+  </si>
+  <si>
+    <t>Xiangping Gao</t>
+  </si>
+  <si>
+    <t>gaoxp@shnu.edu.cn</t>
+  </si>
+  <si>
+    <t>https://osf.io/bw27c</t>
+  </si>
+  <si>
+    <t>Qian et al.</t>
+  </si>
+  <si>
+    <t>Quarterly Journal of Experimental Psychology</t>
+  </si>
+  <si>
+    <t>Qian_2019_QJEP</t>
+  </si>
+  <si>
+    <t>Xiangping Gao
+Haoyue Qian</t>
+  </si>
+  <si>
+    <t>CC-BY-SA 4.0</t>
+  </si>
+  <si>
+    <t>Understanding self-prioritisation: the prioritisation of self-relevant stimuli and its relation to the individual self-esteem</t>
+  </si>
+  <si>
+    <t>Sarah Schäfer and Christian Frings</t>
+  </si>
+  <si>
+    <t>Sarah Schäfer</t>
+  </si>
+  <si>
+    <t>schaefer@psychologie-forum-muenster.de</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.23668/psycharchives.2642</t>
+  </si>
+  <si>
+    <t>Schäfer &amp; Frings</t>
+  </si>
+  <si>
+    <t>Journal of Cognitive Psychology</t>
+  </si>
+  <si>
+    <t>Schaefer_2019_CP</t>
+  </si>
+  <si>
+    <t>Sarah Schäfer
+Marel Pauly
+Dirk Wentura</t>
+  </si>
+  <si>
+    <t>Electrophysiological correlates of self-prioritization</t>
+  </si>
+  <si>
+    <t>Jie Sui,Xun He,Marius Golubickis,Saga L. Svensson,C. Neil Macrae</t>
+  </si>
+  <si>
+    <t>Jie Sui</t>
+  </si>
+  <si>
+    <t>jie.sui@abdn.ac.uk</t>
+  </si>
+  <si>
+    <t>J Sui et al.</t>
+  </si>
+  <si>
+    <t>Sui_2023_CC</t>
+  </si>
+  <si>
+    <t>Sui_2014</t>
+  </si>
+  <si>
+    <t>Unpublish</t>
+  </si>
+  <si>
+    <t>Sui_2015</t>
+  </si>
+  <si>
+    <t>More or less of me and you: self-relevance augments the effects of item probability on stimulus prioritization</t>
+  </si>
+  <si>
+    <t>Saga L. Svensson, Marius Golubickis, Hollie Maclean, Johanna K. Falbén, Linn M. Persson, Dimitra Tsamadi, Siobhan Caughey, Arash Sahraie, C. Neil Macrae</t>
+  </si>
+  <si>
+    <t>Saga L. Svensson</t>
+  </si>
+  <si>
+    <t>s.svensson.19@abdn.ac.uk</t>
+  </si>
+  <si>
+    <t>https://osf.io/cj7fp/</t>
+  </si>
+  <si>
+    <t>Svensson et al.</t>
+  </si>
+  <si>
+    <t>Psychological Research</t>
+  </si>
+  <si>
+    <t>Svensson_2021_PR</t>
+  </si>
+  <si>
+    <t>Towards The Boundaries of Self-Prioritization: Associating The Self With Asymmetric Shapes Disrupts The Self-Prioritization Effect</t>
+  </si>
+  <si>
+    <t>Michele Vicovaro,Mario Dalmaso,Marco Bertamini</t>
+  </si>
+  <si>
+    <t>Michele Vicovaro</t>
+  </si>
+  <si>
+    <t>michele.vicovaro@unipd.it</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.17605/OSF.IO/FE3JW</t>
+  </si>
+  <si>
+    <t>Vicovaro et al.</t>
+  </si>
+  <si>
+    <t>Journal of Experimental Psychology: Human Perception and Performance</t>
+  </si>
+  <si>
+    <t>Vicovaro_2022_EPHPP</t>
+  </si>
+  <si>
+    <t>Mario Dalmaso (Department of Social and Developmental Psychology, University of Padova)
+Marco Bertamini (Department of General Psychology, University of Padova)
+Michele Vicovaro</t>
+  </si>
+  <si>
+    <t>Sarah Schäfer
+Marius Golubickis</t>
+  </si>
+  <si>
+    <t>Prioritization of arbitrary faces associated to self: An EEG study</t>
+  </si>
+  <si>
+    <t>Mateusz Woźniak, Dimitrios Kourtis, Gunther Knoblich</t>
+  </si>
+  <si>
+    <t>Mateusz Wozniak</t>
+  </si>
+  <si>
+    <t>mgwozniak@gmail.com</t>
+  </si>
+  <si>
+    <t>https://journals.plos.org/plosone/article?id=10.1371/journal.pone.0190679#sec025</t>
+  </si>
+  <si>
+    <t>Woźniak et al.</t>
+  </si>
+  <si>
+    <t>PloS one</t>
+  </si>
+  <si>
+    <t>Wozniak_2018_PLOS</t>
+  </si>
+  <si>
+    <t>Stranger to my face: Top-down and bottom-up effects underlying prioritization of images of one’s face</t>
+  </si>
+  <si>
+    <t>Mateusz Woźniak,Jakob Hohwy</t>
+  </si>
+  <si>
+    <t>https://osf.io/2q9w7/</t>
+  </si>
+  <si>
+    <t>PLoS One</t>
+  </si>
+  <si>
+    <t>Wozniak_2020_PLOS</t>
+  </si>
+  <si>
     <t>Self‑prioritization depends on assumed task‑relevance of self‑association</t>
   </si>
   <si>
@@ -666,7 +849,45 @@
     <t>Wozniak_2022_PR</t>
   </si>
   <si>
-    <t>CC BY-NC-ND</t>
+    <t>Romantic feedbacks influence self-relevant processing: the moderating effects of sex difference and facial attractiveness</t>
+  </si>
+  <si>
+    <t>Yang Xu, Yuan Yuan, Xiaochun Xie, Hui Tan, Lili Guan</t>
+  </si>
+  <si>
+    <t>Lili Guan</t>
+  </si>
+  <si>
+    <t>guanll353@nenu.edu.cn</t>
+  </si>
+  <si>
+    <t>Xu et al.</t>
+  </si>
+  <si>
+    <t>Current Psychology</t>
+  </si>
+  <si>
+    <t>Xu_2021_CP</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Template_2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>（未公开数据）</t>
+    </r>
   </si>
   <si>
     <t>Decoding individual differences in self-prioritization from the resting-state functional connectome</t>
@@ -685,143 +906,6 @@
   </si>
   <si>
     <t>Zhang_2023_NI</t>
-  </si>
-  <si>
-    <t>Perceiving the Self and Emotions with an Anxious Mind:Evidence from an Implicit Perceptual Task</t>
-  </si>
-  <si>
-    <t>Michella Feldborg,Naomi A. Lee,Kalai Hung,Kaiping Peng,Jie Sui</t>
-  </si>
-  <si>
-    <t>Kalai Hung</t>
-  </si>
-  <si>
-    <t>hongjl18@mails.tsinghua.edu.cn</t>
-  </si>
-  <si>
-    <t>M Feldborg et al.</t>
-  </si>
-  <si>
-    <t>International Journal of Environmental Research and Public Health</t>
-  </si>
-  <si>
-    <t>Feldborg_2021_ERPH</t>
-  </si>
-  <si>
-    <t>Electrophysiological correlates of self-prioritization</t>
-  </si>
-  <si>
-    <t>Jie Sui,Xun He,Marius Golubickis,Saga L. Svensson,C. Neil Macrae</t>
-  </si>
-  <si>
-    <t>Jie Sui</t>
-  </si>
-  <si>
-    <t>jie.sui@abdn.ac.uk</t>
-  </si>
-  <si>
-    <t>J Sui et al.</t>
-  </si>
-  <si>
-    <t>Consciousness and Cognition</t>
-  </si>
-  <si>
-    <t>Sui_2023_CC</t>
-  </si>
-  <si>
-    <t>Self-prioritization effect in the attentional blink paradigm: Attention-based or familiarity-based effect?</t>
-  </si>
-  <si>
-    <t>Víctor Martínez-Perez,Alejandro Sandoval-Lentisco,Miriam Tortajada,Lucía B. Palmero,Guillermo Campoy,Luis J. Fuentes</t>
-  </si>
-  <si>
-    <t>Luis J. Fuentes</t>
-  </si>
-  <si>
-    <t>lfuentes@um.es</t>
-  </si>
-  <si>
-    <t>https://osf.io/tsvxy/?view_only=4314d303addf4dff9f443bea774a465a</t>
-  </si>
-  <si>
-    <t>V Martínez-Pérez et al.</t>
-  </si>
-  <si>
-    <t>Martinez-Perez_2024_CC</t>
-  </si>
-  <si>
-    <t>Victor Martinez-Perez,
-Lucía B. Palmero,
-Luis J. Fuentes</t>
-  </si>
-  <si>
-    <t>Electrophysiological correlates of self‑related processing in adults with autism</t>
-  </si>
-  <si>
-    <t>Letizia Amodeo,Judith Goris,Annabel D. Nijhof,Jan R. Wiersema</t>
-  </si>
-  <si>
-    <t>Letizia Amodeo</t>
-  </si>
-  <si>
-    <t>letizia.amodeo@ugent.be</t>
-  </si>
-  <si>
-    <t>L Amodeo et al.</t>
-  </si>
-  <si>
-    <t>Cognitive, Affective, &amp; Behavioral Neuroscience</t>
-  </si>
-  <si>
-    <t>Amodeo_2024_CABN</t>
-  </si>
-  <si>
-    <t>Letizia Amodeo
-Judith Goris
-Annabel D. Nijhof
-Jan R. Wiersema</t>
-  </si>
-  <si>
-    <t>Judging me and you: Task design modulates self-prioritization</t>
-  </si>
-  <si>
-    <t>Marius Golubickis,C. Neil Macrae</t>
-  </si>
-  <si>
-    <t>Marius Golubickis</t>
-  </si>
-  <si>
-    <t>marius.golubickis@abdn.ac.uk</t>
-  </si>
-  <si>
-    <t>https://osf.io/8bktn/</t>
-  </si>
-  <si>
-    <t>Golubickis &amp; Macrae</t>
-  </si>
-  <si>
-    <t>Golubickis_2021_AP</t>
-  </si>
-  <si>
-    <t>Socio-cognitive training impacts emotional and perceptual self-salience but not self-other distinction.</t>
-  </si>
-  <si>
-    <t>Henryk Bukowski,Boryana Todorova,Magdalena Boch,Giorgia Silani,Claus Lamm</t>
-  </si>
-  <si>
-    <t>Henryk Bukowski</t>
-  </si>
-  <si>
-    <t>hbbukowski@gmail.com</t>
-  </si>
-  <si>
-    <t>https://osf.io/pcv3u/</t>
-  </si>
-  <si>
-    <t>Henryk Bukowski et al.</t>
-  </si>
-  <si>
-    <t>Bukowski_2021_AP</t>
   </si>
   <si>
     <t>Examining the dorsolateral and ventromedial prefrontal cortex involvement in the self-attention network: A randomized, sham-controlled, parallel group, double-blind, and multichannel HD-tDCS study.</t>
@@ -846,24 +930,6 @@
 Víctor Martínez-Pérez</t>
   </si>
   <si>
-    <t>△</t>
-  </si>
-  <si>
-    <t>Stranger to my face: Top-down and bottom-up effects underlying prioritization of images of one’s face</t>
-  </si>
-  <si>
-    <t>Mateusz Woźniak,Jakob Hohwy</t>
-  </si>
-  <si>
-    <t>https://osf.io/2q9w7/</t>
-  </si>
-  <si>
-    <t>PLoS One</t>
-  </si>
-  <si>
-    <t>Wozniak_2020_PLOS</t>
-  </si>
-  <si>
     <t>△/×</t>
   </si>
   <si>
@@ -894,9 +960,6 @@
     <t>European Journal of Neuroscience</t>
   </si>
   <si>
-    <t>Template_1</t>
-  </si>
-  <si>
     <t>Good Me Bad Me: Prioritization of the Good-Self During Perceptual Decision-Making</t>
   </si>
   <si>
@@ -906,36 +969,6 @@
     <t>Collabra: Psychology</t>
   </si>
   <si>
-    <t>○</t>
-  </si>
-  <si>
-    <t>Relevant for Us? We-Prioritization in Cognitive Processing</t>
-  </si>
-  <si>
-    <t>https://osf.io/sejw7/</t>
-  </si>
-  <si>
-    <t>Journal of Experimental Psychology:  Human Perception and Performance</t>
-  </si>
-  <si>
-    <t>Constable_2019_EPHPP</t>
-  </si>
-  <si>
-    <t>The self can be associated with novel faces of in-group and out-group members: A cross-cultural study</t>
-  </si>
-  <si>
-    <t>Mario Dalmaso</t>
-  </si>
-  <si>
-    <t>mario.dalmaso@unipd.it</t>
-  </si>
-  <si>
-    <t>Mario Dalmaso et al.</t>
-  </si>
-  <si>
-    <t>Dalmaso_2024_CC</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -951,9 +984,6 @@
     <t>Schäfer et al.</t>
   </si>
   <si>
-    <t>Experimental Psychology</t>
-  </si>
-  <si>
     <t>Saliency at first sight: instant identity referential advantage toward a newly met partner</t>
   </si>
   <si>
@@ -988,27 +1018,6 @@
   </si>
   <si>
     <t>Journal of Experimental Psychology:Human Perception and Performance</t>
-  </si>
-  <si>
-    <t>Does Self-Associating a Geometric Shape Immediately Cause Attentional Prioritization?</t>
-  </si>
-  <si>
-    <t>Gabriela Orellana-Corrales, Christina Matschke, Ann-Katrin Wesslein</t>
-  </si>
-  <si>
-    <t>Gabriela Orellana-Corrales</t>
-  </si>
-  <si>
-    <t>gabyorellanac@gmail.com</t>
-  </si>
-  <si>
-    <t>https://osf.io/3ke4f/</t>
-  </si>
-  <si>
-    <t>G Orellana-Corrales et al.</t>
-  </si>
-  <si>
-    <t>Orellana-Corrales_2021_EP</t>
   </si>
 </sst>
 </file>
@@ -1044,9 +1053,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="MyriadPro-Light"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1056,15 +1071,9 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Times New Roman"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="宋体"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="MyriadPro-Light"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1703,11 +1712,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
@@ -1715,13 +1724,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1730,11 +1739,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="6" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2059,15 +2068,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:JO37"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:JO39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="P43" sqref="P43"/>
+      <selection pane="bottomRight" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -2153,7 +2162,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" ht="31" spans="1:275">
+    <row r="2" ht="62" spans="1:275">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2176,14 +2185,14 @@
       <c r="H2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="1" t="s">
         <v>25</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="K2" s="1">
-        <v>2020</v>
+        <v>2024</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>27</v>
@@ -2194,17 +2203,17 @@
       <c r="N2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2" s="7" t="s">
+      <c r="O2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="8" t="s">
         <v>20</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R2" s="1" t="s">
-        <v>23</v>
+      <c r="R2" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -2464,7 +2473,7 @@
       <c r="JN2" s="1"/>
       <c r="JO2" s="1"/>
     </row>
-    <row r="3" ht="46.5" spans="1:275">
+    <row r="3" ht="31" hidden="1" spans="1:275">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2487,14 +2496,14 @@
       <c r="H3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="6" t="s">
         <v>35</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>36</v>
       </c>
       <c r="K3" s="1">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>37</v>
@@ -2505,18 +2514,12 @@
       <c r="N3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="O3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="R3" s="5" t="s">
+      <c r="O3" s="8" t="s">
         <v>40</v>
       </c>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
@@ -2775,28 +2778,24 @@
       <c r="JN3" s="1"/>
       <c r="JO3" s="1"/>
     </row>
-    <row r="4" ht="31" spans="1:275">
+    <row r="4" ht="15.5" spans="1:275">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="C4" s="3"/>
       <c r="D4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="5"/>
+      <c r="G4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>44</v>
@@ -2805,7 +2804,7 @@
         <v>45</v>
       </c>
       <c r="K4" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>46</v>
@@ -2814,20 +2813,16 @@
         <v>47</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O4" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>23</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
@@ -3098,18 +3093,18 @@
         <v>20</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I5" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>52</v>
       </c>
       <c r="J5" s="1" t="s">
@@ -3119,25 +3114,25 @@
         <v>2020</v>
       </c>
       <c r="L5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O5" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="P5" s="7" t="s">
+      <c r="O5" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="P5" s="8" t="s">
         <v>20</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R5" s="5" t="s">
-        <v>56</v>
+      <c r="R5" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -3397,13 +3392,11 @@
       <c r="JN5" s="1"/>
       <c r="JO5" s="1"/>
     </row>
-    <row r="6" ht="46.5" spans="1:275">
+    <row r="6" ht="31" spans="1:275">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>57</v>
-      </c>
+      <c r="B6" s="1"/>
       <c r="C6" s="3" t="s">
         <v>20</v>
       </c>
@@ -3411,46 +3404,46 @@
         <v>20</v>
       </c>
       <c r="E6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="H6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="J6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="1">
+        <v>2020</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="M6" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I6" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="K6" s="1">
-        <v>2019</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="N6" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="P6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="P6" s="8" t="s">
         <v>20</v>
       </c>
       <c r="Q6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R6" s="5" t="s">
-        <v>67</v>
+      <c r="R6" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="S6" s="1"/>
       <c r="T6" s="5"/>
@@ -3714,60 +3707,52 @@
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>20</v>
+      <c r="B7" s="1"/>
+      <c r="C7" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>70</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="F7" s="5"/>
       <c r="G7" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>73</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="K7" s="1">
-        <v>2018</v>
+        <v>2024</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="P7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>71</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q7" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="R7" s="1"/>
       <c r="S7" s="1"/>
       <c r="T7" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
@@ -4030,7 +4015,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>20</v>
@@ -4038,45 +4023,47 @@
       <c r="D8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>80</v>
+      <c r="E8" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>72</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>83</v>
+        <v>74</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="K8" s="1">
         <v>2021</v>
       </c>
-      <c r="L8" s="1"/>
+      <c r="L8" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="M8" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="O8" s="7" t="s">
+      <c r="O8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="P8" s="7" t="s">
-        <v>20</v>
+      <c r="P8" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="Q8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R8" s="5" t="s">
-        <v>86</v>
+      <c r="R8" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
@@ -4336,11 +4323,13 @@
       <c r="JN8" s="1"/>
       <c r="JO8" s="1"/>
     </row>
-    <row r="9" ht="46.5" spans="1:275">
+    <row r="9" ht="15.5" hidden="1" spans="1:275">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="9" t="s">
+        <v>79</v>
+      </c>
       <c r="C9" s="3" t="s">
         <v>20</v>
       </c>
@@ -4348,37 +4337,37 @@
         <v>20</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>91</v>
+        <v>83</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>84</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K9" s="1">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>93</v>
+        <v>37</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="O9" s="7" t="s">
-        <v>30</v>
+      <c r="O9" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
@@ -4641,11 +4630,13 @@
       <c r="JN9" s="1"/>
       <c r="JO9" s="1"/>
     </row>
-    <row r="10" ht="31" spans="1:275">
+    <row r="10" ht="46.5" spans="1:275">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="C10" s="3" t="s">
         <v>20</v>
       </c>
@@ -4653,46 +4644,46 @@
         <v>20</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>35</v>
+        <v>90</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>91</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="K10" s="1">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="O10" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="O10" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="P10" s="7" t="s">
+      <c r="P10" s="8" t="s">
         <v>20</v>
       </c>
       <c r="Q10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R10" s="1" t="s">
-        <v>97</v>
+      <c r="R10" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
@@ -4952,7 +4943,7 @@
       <c r="JN10" s="1"/>
       <c r="JO10" s="1"/>
     </row>
-    <row r="11" ht="31" spans="1:275">
+    <row r="11" ht="31" hidden="1" spans="1:275">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -4963,48 +4954,42 @@
       <c r="D11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>104</v>
+      <c r="E11" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>97</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>107</v>
+        <v>99</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>100</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="K11" s="1">
         <v>2023</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="O11" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="P11" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>20</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="O11" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
@@ -5274,39 +5259,39 @@
       <c r="D12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>114</v>
+      <c r="E12" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>105</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="K12" s="1">
         <v>2023</v>
       </c>
       <c r="L12" s="1"/>
       <c r="M12" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="O12" s="7" t="s">
+      <c r="O12" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="P12" s="7" t="s">
-        <v>112</v>
+      <c r="P12" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="Q12" s="1" t="s">
         <v>20</v>
@@ -5576,9 +5561,7 @@
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>68</v>
-      </c>
+      <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
         <v>20</v>
       </c>
@@ -5586,46 +5569,46 @@
         <v>20</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>124</v>
+        <v>115</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="K13" s="1">
-        <v>2023</v>
+        <v>2020</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="O13" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="P13" s="7" t="s">
+      <c r="P13" s="8" t="s">
         <v>20</v>
       </c>
       <c r="Q13" s="1" t="s">
         <v>20</v>
       </c>
       <c r="R13" s="5" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
@@ -5896,42 +5879,48 @@
       <c r="D14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>130</v>
+      <c r="E14" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>121</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="I14" s="15" t="s">
-        <v>133</v>
+        <v>123</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>124</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="K14" s="1">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O14" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="O14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="P14" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
@@ -6201,41 +6190,41 @@
       <c r="D15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>138</v>
+      <c r="E15" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>128</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="K15" s="1">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>37</v>
+        <v>133</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O15" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="O15" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="P15" s="7" t="s">
-        <v>112</v>
+      <c r="P15" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="Q15" s="1" t="s">
         <v>20</v>
@@ -6506,7 +6495,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>20</v>
@@ -6515,52 +6504,50 @@
         <v>20</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>146</v>
+        <v>136</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>137</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="K16" s="1">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>150</v>
+        <v>67</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O16" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="O16" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="P16" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="P16" s="7" t="s">
+      <c r="Q16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Q16" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="R16" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="S16" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="T16" s="16" t="s">
-        <v>154</v>
+        <v>142</v>
+      </c>
+      <c r="S16" s="1"/>
+      <c r="T16" s="17" t="s">
+        <v>143</v>
       </c>
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
@@ -6823,7 +6810,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>68</v>
+        <v>144</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>20</v>
@@ -6832,43 +6819,45 @@
         <v>20</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>157</v>
+        <v>146</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="K17" s="1">
-        <v>2022</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>161</v>
-      </c>
+        <v>2021</v>
+      </c>
+      <c r="L17" s="1"/>
       <c r="M17" s="1" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O17" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="P17" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="O17" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
+      <c r="P17" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R17" s="5" t="s">
+        <v>152</v>
+      </c>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
@@ -7127,61 +7116,53 @@
       <c r="JN17" s="1"/>
       <c r="JO17" s="1"/>
     </row>
-    <row r="18" ht="31" spans="1:275">
+    <row r="18" ht="31" hidden="1" spans="1:275">
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>20</v>
+      <c r="B18" s="1"/>
+      <c r="C18" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>71</v>
+        <v>155</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>72</v>
+        <v>156</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>74</v>
+        <v>158</v>
       </c>
       <c r="K18" s="1">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>93</v>
+        <v>159</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O18" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="P18" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="R18" s="1" t="s">
-        <v>71</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="O18" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
@@ -7445,7 +7426,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>167</v>
+        <v>70</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>20</v>
@@ -7453,48 +7434,44 @@
       <c r="D19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="K19" s="1">
+        <v>2022</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="M19" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="F19" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="K19" s="1">
-        <v>2023</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>173</v>
-      </c>
       <c r="N19" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O19" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="O19" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="P19" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="P19" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="R19" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
@@ -7757,56 +7734,54 @@
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>68</v>
-      </c>
+      <c r="B20" s="1"/>
       <c r="C20" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="K20" s="1">
+        <v>2020</v>
+      </c>
+      <c r="L20" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="M20" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="H20" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="K20" s="1">
-        <v>2021</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>180</v>
-      </c>
       <c r="N20" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O20" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="O20" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="P20" s="7" t="s">
-        <v>112</v>
+      <c r="P20" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="Q20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R20" s="1" t="s">
-        <v>20</v>
+      <c r="R20" s="5" t="s">
+        <v>177</v>
       </c>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
@@ -8066,12 +8041,12 @@
       <c r="JN20" s="1"/>
       <c r="JO20" s="1"/>
     </row>
-    <row r="21" ht="15.5" spans="1:275">
+    <row r="21" ht="46.5" spans="1:275">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>20</v>
@@ -8079,47 +8054,47 @@
       <c r="D21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="H21" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="G21" s="9" t="s">
+      <c r="I21" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="J21" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="I21" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J21" s="1" t="s">
+      <c r="K21" s="1">
+        <v>2019</v>
+      </c>
+      <c r="L21" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="K21" s="1">
-        <v>2023</v>
-      </c>
-      <c r="L21" s="1" t="s">
+      <c r="M21" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="M21" s="1" t="s">
-        <v>187</v>
-      </c>
       <c r="N21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O21" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="O21" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="P21" s="7" t="s">
-        <v>112</v>
+      <c r="P21" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="Q21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R21" s="1" t="s">
-        <v>20</v>
+      <c r="R21" s="5" t="s">
+        <v>187</v>
       </c>
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
@@ -8379,12 +8354,12 @@
       <c r="JN21" s="1"/>
       <c r="JO21" s="1"/>
     </row>
-    <row r="22" ht="46.5" spans="1:275">
+    <row r="22" ht="15.5" spans="1:275">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>20</v>
@@ -8392,47 +8367,47 @@
       <c r="D22" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="G22" s="10" t="s">
         <v>190</v>
       </c>
       <c r="H22" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="I22" s="6" t="s">
+      <c r="I22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J22" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="K22" s="1">
+        <v>2023</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M22" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="K22" s="1">
-        <v>2024</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>194</v>
-      </c>
       <c r="N22" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O22" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="P22" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="O22" s="8" t="s">
         <v>20</v>
+      </c>
+      <c r="P22" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="Q22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R22" s="5" t="s">
-        <v>195</v>
+      <c r="R22" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
@@ -8692,59 +8667,39 @@
       <c r="JN22" s="1"/>
       <c r="JO22" s="1"/>
     </row>
-    <row r="23" ht="62" spans="1:275">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
+    <row r="23" ht="15.5" spans="1:275">
+      <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="4"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1">
+        <v>2014</v>
+      </c>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="O23" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="K23" s="1">
-        <v>2024</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O23" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="P23" s="7" t="s">
-        <v>20</v>
+      <c r="P23" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="Q23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R23" s="5" t="s">
-        <v>203</v>
-      </c>
+      <c r="R23" s="1"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
@@ -9004,53 +8959,37 @@
       <c r="JO23" s="1"/>
     </row>
     <row r="24" ht="15.5" spans="1:275">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>167</v>
-      </c>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
       <c r="C24" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="4"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1">
+        <v>2015</v>
+      </c>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="O24" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="I24" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="K24" s="1">
-        <v>2021</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O24" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
+      <c r="P24" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
@@ -9310,9 +9249,9 @@
       <c r="JN24" s="1"/>
       <c r="JO24" s="1"/>
     </row>
-    <row r="25" ht="31" spans="1:275">
+    <row r="25" ht="46.5" hidden="1" spans="1:275">
       <c r="A25" s="1">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="3" t="s">
@@ -9322,37 +9261,37 @@
         <v>20</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="K25" s="1">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O25" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="O25" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
@@ -9615,50 +9554,64 @@
       <c r="JN25" s="1"/>
       <c r="JO25" s="1"/>
     </row>
-    <row r="26" ht="62" spans="1:275">
+    <row r="26" ht="46.5" spans="1:275">
       <c r="A26" s="1">
-        <v>25</v>
-      </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="E26" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="F26" s="5"/>
+        <v>205</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>206</v>
+      </c>
       <c r="G26" s="1" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="K26" s="1">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="M26" s="1"/>
+        <v>211</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="N26" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="O26" s="7" t="s">
+      <c r="O26" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="P26" s="7" t="s">
+      <c r="P26" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="Q26" s="1"/>
+      <c r="Q26" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="R26" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="S26" s="1"/>
+        <v>213</v>
+      </c>
+      <c r="S26" s="5" t="s">
+        <v>214</v>
+      </c>
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
       <c r="V26" s="1"/>
@@ -9916,57 +9869,61 @@
       <c r="JN26" s="1"/>
       <c r="JO26" s="1"/>
     </row>
-    <row r="27" ht="31" spans="1:275">
+    <row r="27" ht="15.5" spans="1:275">
       <c r="A27" s="1">
-        <v>26</v>
-      </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="11" t="s">
-        <v>225</v>
+        <v>24</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>71</v>
+        <v>217</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>72</v>
+        <v>218</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>74</v>
+        <v>220</v>
       </c>
       <c r="K27" s="1">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O27" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="P27" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="Q27" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="R27" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="O27" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="P27" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
@@ -10225,42 +10182,56 @@
       <c r="JN27" s="1"/>
       <c r="JO27" s="1"/>
     </row>
-    <row r="28" ht="15.5" spans="1:275">
+    <row r="28" ht="31" spans="1:275">
       <c r="A28" s="1">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B28" s="1"/>
-      <c r="C28" s="11" t="s">
-        <v>231</v>
+      <c r="C28" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>232</v>
+        <v>20</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="F28" s="5"/>
+        <v>223</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>224</v>
+      </c>
       <c r="G28" s="1" t="s">
-        <v>71</v>
+        <v>217</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="10" t="s">
-        <v>234</v>
-      </c>
-      <c r="O28" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="I28" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="P28" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="Q28" s="1"/>
+      <c r="J28" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="K28" s="1">
+        <v>2020</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O28" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="P28" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q28" s="16" t="s">
+        <v>62</v>
+      </c>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
@@ -10522,45 +10493,59 @@
     </row>
     <row r="29" ht="31" spans="1:275">
       <c r="A29" s="1">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C29" s="3"/>
+        <v>70</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="D29" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="F29" s="5"/>
+        <v>228</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>229</v>
+      </c>
       <c r="G29" s="1" t="s">
-        <v>236</v>
+        <v>217</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>237</v>
+        <v>218</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>239</v>
+        <v>220</v>
       </c>
       <c r="K29" s="1">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="M29" s="1"/>
+        <v>203</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>231</v>
+      </c>
       <c r="N29" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="O29" s="7"/>
-      <c r="P29" s="7"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="O29" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="P29" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
       <c r="U29" s="1"/>
@@ -10821,47 +10806,57 @@
     </row>
     <row r="30" ht="31" spans="1:275">
       <c r="A30" s="1">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B30" s="1"/>
-      <c r="C30" s="3"/>
+      <c r="C30" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="D30" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E30" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="F30" s="7"/>
+      <c r="E30" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>233</v>
+      </c>
       <c r="G30" s="1" t="s">
-        <v>115</v>
+        <v>234</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="I30" s="6" t="s">
-        <v>243</v>
+        <v>235</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>118</v>
+        <v>236</v>
       </c>
       <c r="K30" s="1">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M30" s="1"/>
+        <v>237</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>238</v>
+      </c>
       <c r="N30" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="O30" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="P30" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="Q30" s="1"/>
-      <c r="R30" s="1"/>
+        <v>239</v>
+      </c>
+      <c r="O30" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="P30" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R30" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
@@ -11120,51 +11115,61 @@
       <c r="JN30" s="1"/>
       <c r="JO30" s="1"/>
     </row>
-    <row r="31" ht="15.5" spans="1:275">
+    <row r="31" ht="31" spans="1:275">
       <c r="A31" s="1">
-        <v>30</v>
-      </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="D31" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E31" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="F31" s="5"/>
-      <c r="G31" s="1" t="s">
-        <v>23</v>
+      <c r="E31" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>122</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>24</v>
+        <v>123</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>45</v>
+        <v>243</v>
       </c>
       <c r="K31" s="1">
-        <v>2019</v>
+        <v>2023</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="O31" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="P31" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="Q31" s="1"/>
-      <c r="R31" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="O31" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="P31" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
@@ -11423,53 +11428,49 @@
       <c r="JN31" s="1"/>
       <c r="JO31" s="1"/>
     </row>
-    <row r="32" ht="31" spans="1:275">
+    <row r="32" ht="62" spans="1:275">
       <c r="A32" s="1">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B32" s="1"/>
-      <c r="C32" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="4"/>
       <c r="E32" s="5" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="K32" s="1">
+        <v>2020</v>
+      </c>
+      <c r="L32" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="H32" s="6" t="s">
+      <c r="M32" s="1"/>
+      <c r="N32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O32" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="P32" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="K32" s="1">
-        <v>2024</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="N32" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O32" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="P32" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="Q32" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="R32" s="1"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
@@ -11728,46 +11729,40 @@
       <c r="JN32" s="1"/>
       <c r="JO32" s="1"/>
     </row>
-    <row r="33" ht="31" spans="1:275">
+    <row r="33" ht="15.5" spans="1:275">
       <c r="A33" s="1">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B33" s="1"/>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>255</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>256</v>
       </c>
       <c r="F33" s="5"/>
       <c r="G33" s="1" t="s">
-        <v>257</v>
+        <v>217</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="K33" s="1">
-        <v>2023</v>
-      </c>
-      <c r="L33" s="1" t="s">
-        <v>260</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
       <c r="M33" s="1"/>
-      <c r="N33" s="10" t="s">
-        <v>234</v>
-      </c>
-      <c r="O33" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="P33" s="7" t="s">
-        <v>232</v>
+      <c r="N33" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="O33" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="P33" s="8" t="s">
+        <v>254</v>
       </c>
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
@@ -12029,35 +12024,45 @@
       <c r="JN33" s="1"/>
       <c r="JO33" s="1"/>
     </row>
-    <row r="34" ht="31" spans="1:275">
+    <row r="34" ht="31" hidden="1" spans="1:275">
       <c r="A34" s="1">
-        <v>33</v>
-      </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="3" t="s">
-        <v>255</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="3"/>
       <c r="D34" s="4" t="s">
-        <v>232</v>
+        <v>20</v>
       </c>
       <c r="E34" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="F34" s="5"/>
+      <c r="G34" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="J34" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="F34" s="5"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="6" t="s">
+      <c r="K34" s="1">
+        <v>2021</v>
+      </c>
+      <c r="L34" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
       <c r="M34" s="1"/>
-      <c r="N34" s="10" t="s">
-        <v>263</v>
-      </c>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
+      <c r="N34" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
@@ -12320,37 +12325,45 @@
     </row>
     <row r="35" ht="31" spans="1:275">
       <c r="A35" s="1">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5" t="s">
+      <c r="C35" s="3"/>
+      <c r="D35" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="F35" s="8"/>
+      <c r="G35" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="I35" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="F35" s="5"/>
-      <c r="G35" s="1" t="s">
+      <c r="J35" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K35" s="1">
+        <v>2020</v>
+      </c>
+      <c r="L35" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>266</v>
-      </c>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="K35" s="1">
-        <v>2024</v>
-      </c>
-      <c r="L35" s="1" t="s">
-        <v>268</v>
       </c>
       <c r="M35" s="1"/>
       <c r="N35" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
+        <v>111</v>
+      </c>
+      <c r="O35" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="P35" s="8" t="s">
+        <v>49</v>
+      </c>
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
@@ -12613,37 +12626,45 @@
     </row>
     <row r="36" ht="31" spans="1:275">
       <c r="A36" s="1">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="5"/>
+      <c r="C36" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>254</v>
+      </c>
       <c r="E36" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="F36" s="5"/>
+      <c r="G36" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="H36" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="F36" s="5"/>
-      <c r="G36" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="H36" s="6" t="s">
+      <c r="I36" s="9"/>
+      <c r="J36" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1" t="s">
-        <v>271</v>
-      </c>
       <c r="K36" s="1">
-        <v>2016</v>
+        <v>2023</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>272</v>
+        <v>159</v>
       </c>
       <c r="M36" s="1"/>
-      <c r="N36" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="O36" s="1"/>
-      <c r="P36" s="1"/>
+      <c r="N36" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="O36" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="P36" s="8" t="s">
+        <v>254</v>
+      </c>
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
@@ -12904,50 +12925,34 @@
       <c r="JN36" s="1"/>
       <c r="JO36" s="1"/>
     </row>
-    <row r="37" ht="31" spans="1:275">
+    <row r="37" ht="31" hidden="1" spans="1:275">
       <c r="A37" s="1">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B37" s="1"/>
-      <c r="C37" s="13" t="s">
-        <v>245</v>
+      <c r="C37" s="3" t="s">
+        <v>266</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>20</v>
+        <v>254</v>
       </c>
       <c r="E37" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="F37" s="5"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="F37" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="I37" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="J37" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="K37" s="1">
-        <v>2020</v>
-      </c>
-      <c r="L37" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="M37" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="N37" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="O37" s="7" t="s">
-        <v>245</v>
-      </c>
+      <c r="O37" s="1"/>
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
@@ -13209,69 +13214,667 @@
       <c r="JN37" s="1"/>
       <c r="JO37" s="1"/>
     </row>
+    <row r="38" ht="31" hidden="1" spans="1:275">
+      <c r="A38" s="1">
+        <v>35</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="F38" s="5"/>
+      <c r="G38" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="K38" s="1">
+        <v>2024</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
+      <c r="T38" s="1"/>
+      <c r="U38" s="1"/>
+      <c r="V38" s="1"/>
+      <c r="W38" s="1"/>
+      <c r="X38" s="1"/>
+      <c r="Y38" s="1"/>
+      <c r="Z38" s="1"/>
+      <c r="AA38" s="1"/>
+      <c r="AB38" s="1"/>
+      <c r="AC38" s="1"/>
+      <c r="AD38" s="1"/>
+      <c r="AE38" s="1"/>
+      <c r="AF38" s="1"/>
+      <c r="AG38" s="1"/>
+      <c r="AH38" s="1"/>
+      <c r="AI38" s="1"/>
+      <c r="AJ38" s="1"/>
+      <c r="AK38" s="1"/>
+      <c r="AL38" s="1"/>
+      <c r="AM38" s="1"/>
+      <c r="AN38" s="1"/>
+      <c r="AO38" s="1"/>
+      <c r="AP38" s="1"/>
+      <c r="AQ38" s="1"/>
+      <c r="AR38" s="1"/>
+      <c r="AS38" s="1"/>
+      <c r="AT38" s="1"/>
+      <c r="AU38" s="1"/>
+      <c r="AV38" s="1"/>
+      <c r="AW38" s="1"/>
+      <c r="AX38" s="1"/>
+      <c r="AY38" s="1"/>
+      <c r="AZ38" s="1"/>
+      <c r="BA38" s="1"/>
+      <c r="BB38" s="1"/>
+      <c r="BC38" s="1"/>
+      <c r="BD38" s="1"/>
+      <c r="BE38" s="1"/>
+      <c r="BF38" s="1"/>
+      <c r="BG38" s="1"/>
+      <c r="BH38" s="1"/>
+      <c r="BI38" s="1"/>
+      <c r="BJ38" s="1"/>
+      <c r="BK38" s="1"/>
+      <c r="BL38" s="1"/>
+      <c r="BM38" s="1"/>
+      <c r="BN38" s="1"/>
+      <c r="BO38" s="1"/>
+      <c r="BP38" s="1"/>
+      <c r="BQ38" s="1"/>
+      <c r="BR38" s="1"/>
+      <c r="BS38" s="1"/>
+      <c r="BT38" s="1"/>
+      <c r="BU38" s="1"/>
+      <c r="BV38" s="1"/>
+      <c r="BW38" s="1"/>
+      <c r="BX38" s="1"/>
+      <c r="BY38" s="1"/>
+      <c r="BZ38" s="1"/>
+      <c r="CA38" s="1"/>
+      <c r="CB38" s="1"/>
+      <c r="CC38" s="1"/>
+      <c r="CD38" s="1"/>
+      <c r="CE38" s="1"/>
+      <c r="CF38" s="1"/>
+      <c r="CG38" s="1"/>
+      <c r="CH38" s="1"/>
+      <c r="CI38" s="1"/>
+      <c r="CJ38" s="1"/>
+      <c r="CK38" s="1"/>
+      <c r="CL38" s="1"/>
+      <c r="CM38" s="1"/>
+      <c r="CN38" s="1"/>
+      <c r="CO38" s="1"/>
+      <c r="CP38" s="1"/>
+      <c r="CQ38" s="1"/>
+      <c r="CR38" s="1"/>
+      <c r="CS38" s="1"/>
+      <c r="CT38" s="1"/>
+      <c r="CU38" s="1"/>
+      <c r="CV38" s="1"/>
+      <c r="CW38" s="1"/>
+      <c r="CX38" s="1"/>
+      <c r="CY38" s="1"/>
+      <c r="CZ38" s="1"/>
+      <c r="DA38" s="1"/>
+      <c r="DB38" s="1"/>
+      <c r="DC38" s="1"/>
+      <c r="DD38" s="1"/>
+      <c r="DE38" s="1"/>
+      <c r="DF38" s="1"/>
+      <c r="DG38" s="1"/>
+      <c r="DH38" s="1"/>
+      <c r="DI38" s="1"/>
+      <c r="DJ38" s="1"/>
+      <c r="DK38" s="1"/>
+      <c r="DL38" s="1"/>
+      <c r="DM38" s="1"/>
+      <c r="DN38" s="1"/>
+      <c r="DO38" s="1"/>
+      <c r="DP38" s="1"/>
+      <c r="DQ38" s="1"/>
+      <c r="DR38" s="1"/>
+      <c r="DS38" s="1"/>
+      <c r="DT38" s="1"/>
+      <c r="DU38" s="1"/>
+      <c r="DV38" s="1"/>
+      <c r="DW38" s="1"/>
+      <c r="DX38" s="1"/>
+      <c r="DY38" s="1"/>
+      <c r="DZ38" s="1"/>
+      <c r="EA38" s="1"/>
+      <c r="EB38" s="1"/>
+      <c r="EC38" s="1"/>
+      <c r="ED38" s="1"/>
+      <c r="EE38" s="1"/>
+      <c r="EF38" s="1"/>
+      <c r="EG38" s="1"/>
+      <c r="EH38" s="1"/>
+      <c r="EI38" s="1"/>
+      <c r="EJ38" s="1"/>
+      <c r="EK38" s="1"/>
+      <c r="EL38" s="1"/>
+      <c r="EM38" s="1"/>
+      <c r="EN38" s="1"/>
+      <c r="EO38" s="1"/>
+      <c r="EP38" s="1"/>
+      <c r="EQ38" s="1"/>
+      <c r="ER38" s="1"/>
+      <c r="ES38" s="1"/>
+      <c r="ET38" s="1"/>
+      <c r="EU38" s="1"/>
+      <c r="EV38" s="1"/>
+      <c r="EW38" s="1"/>
+      <c r="EX38" s="1"/>
+      <c r="EY38" s="1"/>
+      <c r="EZ38" s="1"/>
+      <c r="FA38" s="1"/>
+      <c r="FB38" s="1"/>
+      <c r="FC38" s="1"/>
+      <c r="FD38" s="1"/>
+      <c r="FE38" s="1"/>
+      <c r="FF38" s="1"/>
+      <c r="FG38" s="1"/>
+      <c r="FH38" s="1"/>
+      <c r="FI38" s="1"/>
+      <c r="FJ38" s="1"/>
+      <c r="FK38" s="1"/>
+      <c r="FL38" s="1"/>
+      <c r="FM38" s="1"/>
+      <c r="FN38" s="1"/>
+      <c r="FO38" s="1"/>
+      <c r="FP38" s="1"/>
+      <c r="FQ38" s="1"/>
+      <c r="FR38" s="1"/>
+      <c r="FS38" s="1"/>
+      <c r="FT38" s="1"/>
+      <c r="FU38" s="1"/>
+      <c r="FV38" s="1"/>
+      <c r="FW38" s="1"/>
+      <c r="FX38" s="1"/>
+      <c r="FY38" s="1"/>
+      <c r="FZ38" s="1"/>
+      <c r="GA38" s="1"/>
+      <c r="GB38" s="1"/>
+      <c r="GC38" s="1"/>
+      <c r="GD38" s="1"/>
+      <c r="GE38" s="1"/>
+      <c r="GF38" s="1"/>
+      <c r="GG38" s="1"/>
+      <c r="GH38" s="1"/>
+      <c r="GI38" s="1"/>
+      <c r="GJ38" s="1"/>
+      <c r="GK38" s="1"/>
+      <c r="GL38" s="1"/>
+      <c r="GM38" s="1"/>
+      <c r="GN38" s="1"/>
+      <c r="GO38" s="1"/>
+      <c r="GP38" s="1"/>
+      <c r="GQ38" s="1"/>
+      <c r="GR38" s="1"/>
+      <c r="GS38" s="1"/>
+      <c r="GT38" s="1"/>
+      <c r="GU38" s="1"/>
+      <c r="GV38" s="1"/>
+      <c r="GW38" s="1"/>
+      <c r="GX38" s="1"/>
+      <c r="GY38" s="1"/>
+      <c r="GZ38" s="1"/>
+      <c r="HA38" s="1"/>
+      <c r="HB38" s="1"/>
+      <c r="HC38" s="1"/>
+      <c r="HD38" s="1"/>
+      <c r="HE38" s="1"/>
+      <c r="HF38" s="1"/>
+      <c r="HG38" s="1"/>
+      <c r="HH38" s="1"/>
+      <c r="HI38" s="1"/>
+      <c r="HJ38" s="1"/>
+      <c r="HK38" s="1"/>
+      <c r="HL38" s="1"/>
+      <c r="HM38" s="1"/>
+      <c r="HN38" s="1"/>
+      <c r="HO38" s="1"/>
+      <c r="HP38" s="1"/>
+      <c r="HQ38" s="1"/>
+      <c r="HR38" s="1"/>
+      <c r="HS38" s="1"/>
+      <c r="HT38" s="1"/>
+      <c r="HU38" s="1"/>
+      <c r="HV38" s="1"/>
+      <c r="HW38" s="1"/>
+      <c r="HX38" s="1"/>
+      <c r="HY38" s="1"/>
+      <c r="HZ38" s="1"/>
+      <c r="IA38" s="1"/>
+      <c r="IB38" s="1"/>
+      <c r="IC38" s="1"/>
+      <c r="ID38" s="1"/>
+      <c r="IE38" s="1"/>
+      <c r="IF38" s="1"/>
+      <c r="IG38" s="1"/>
+      <c r="IH38" s="1"/>
+      <c r="II38" s="1"/>
+      <c r="IJ38" s="1"/>
+      <c r="IK38" s="1"/>
+      <c r="IL38" s="1"/>
+      <c r="IM38" s="1"/>
+      <c r="IN38" s="1"/>
+      <c r="IO38" s="1"/>
+      <c r="IP38" s="1"/>
+      <c r="IQ38" s="1"/>
+      <c r="IR38" s="1"/>
+      <c r="IS38" s="1"/>
+      <c r="IT38" s="1"/>
+      <c r="IU38" s="1"/>
+      <c r="IV38" s="1"/>
+      <c r="IW38" s="1"/>
+      <c r="IX38" s="1"/>
+      <c r="IY38" s="1"/>
+      <c r="IZ38" s="1"/>
+      <c r="JA38" s="1"/>
+      <c r="JB38" s="1"/>
+      <c r="JC38" s="1"/>
+      <c r="JD38" s="1"/>
+      <c r="JE38" s="1"/>
+      <c r="JF38" s="1"/>
+      <c r="JG38" s="1"/>
+      <c r="JH38" s="1"/>
+      <c r="JI38" s="1"/>
+      <c r="JJ38" s="1"/>
+      <c r="JK38" s="1"/>
+      <c r="JL38" s="1"/>
+      <c r="JM38" s="1"/>
+      <c r="JN38" s="1"/>
+      <c r="JO38" s="1"/>
+    </row>
+    <row r="39" ht="31" hidden="1" spans="1:275">
+      <c r="A39" s="1">
+        <v>36</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="F39" s="5"/>
+      <c r="G39" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="K39" s="1">
+        <v>2016</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1"/>
+      <c r="T39" s="1"/>
+      <c r="U39" s="1"/>
+      <c r="V39" s="1"/>
+      <c r="W39" s="1"/>
+      <c r="X39" s="1"/>
+      <c r="Y39" s="1"/>
+      <c r="Z39" s="1"/>
+      <c r="AA39" s="1"/>
+      <c r="AB39" s="1"/>
+      <c r="AC39" s="1"/>
+      <c r="AD39" s="1"/>
+      <c r="AE39" s="1"/>
+      <c r="AF39" s="1"/>
+      <c r="AG39" s="1"/>
+      <c r="AH39" s="1"/>
+      <c r="AI39" s="1"/>
+      <c r="AJ39" s="1"/>
+      <c r="AK39" s="1"/>
+      <c r="AL39" s="1"/>
+      <c r="AM39" s="1"/>
+      <c r="AN39" s="1"/>
+      <c r="AO39" s="1"/>
+      <c r="AP39" s="1"/>
+      <c r="AQ39" s="1"/>
+      <c r="AR39" s="1"/>
+      <c r="AS39" s="1"/>
+      <c r="AT39" s="1"/>
+      <c r="AU39" s="1"/>
+      <c r="AV39" s="1"/>
+      <c r="AW39" s="1"/>
+      <c r="AX39" s="1"/>
+      <c r="AY39" s="1"/>
+      <c r="AZ39" s="1"/>
+      <c r="BA39" s="1"/>
+      <c r="BB39" s="1"/>
+      <c r="BC39" s="1"/>
+      <c r="BD39" s="1"/>
+      <c r="BE39" s="1"/>
+      <c r="BF39" s="1"/>
+      <c r="BG39" s="1"/>
+      <c r="BH39" s="1"/>
+      <c r="BI39" s="1"/>
+      <c r="BJ39" s="1"/>
+      <c r="BK39" s="1"/>
+      <c r="BL39" s="1"/>
+      <c r="BM39" s="1"/>
+      <c r="BN39" s="1"/>
+      <c r="BO39" s="1"/>
+      <c r="BP39" s="1"/>
+      <c r="BQ39" s="1"/>
+      <c r="BR39" s="1"/>
+      <c r="BS39" s="1"/>
+      <c r="BT39" s="1"/>
+      <c r="BU39" s="1"/>
+      <c r="BV39" s="1"/>
+      <c r="BW39" s="1"/>
+      <c r="BX39" s="1"/>
+      <c r="BY39" s="1"/>
+      <c r="BZ39" s="1"/>
+      <c r="CA39" s="1"/>
+      <c r="CB39" s="1"/>
+      <c r="CC39" s="1"/>
+      <c r="CD39" s="1"/>
+      <c r="CE39" s="1"/>
+      <c r="CF39" s="1"/>
+      <c r="CG39" s="1"/>
+      <c r="CH39" s="1"/>
+      <c r="CI39" s="1"/>
+      <c r="CJ39" s="1"/>
+      <c r="CK39" s="1"/>
+      <c r="CL39" s="1"/>
+      <c r="CM39" s="1"/>
+      <c r="CN39" s="1"/>
+      <c r="CO39" s="1"/>
+      <c r="CP39" s="1"/>
+      <c r="CQ39" s="1"/>
+      <c r="CR39" s="1"/>
+      <c r="CS39" s="1"/>
+      <c r="CT39" s="1"/>
+      <c r="CU39" s="1"/>
+      <c r="CV39" s="1"/>
+      <c r="CW39" s="1"/>
+      <c r="CX39" s="1"/>
+      <c r="CY39" s="1"/>
+      <c r="CZ39" s="1"/>
+      <c r="DA39" s="1"/>
+      <c r="DB39" s="1"/>
+      <c r="DC39" s="1"/>
+      <c r="DD39" s="1"/>
+      <c r="DE39" s="1"/>
+      <c r="DF39" s="1"/>
+      <c r="DG39" s="1"/>
+      <c r="DH39" s="1"/>
+      <c r="DI39" s="1"/>
+      <c r="DJ39" s="1"/>
+      <c r="DK39" s="1"/>
+      <c r="DL39" s="1"/>
+      <c r="DM39" s="1"/>
+      <c r="DN39" s="1"/>
+      <c r="DO39" s="1"/>
+      <c r="DP39" s="1"/>
+      <c r="DQ39" s="1"/>
+      <c r="DR39" s="1"/>
+      <c r="DS39" s="1"/>
+      <c r="DT39" s="1"/>
+      <c r="DU39" s="1"/>
+      <c r="DV39" s="1"/>
+      <c r="DW39" s="1"/>
+      <c r="DX39" s="1"/>
+      <c r="DY39" s="1"/>
+      <c r="DZ39" s="1"/>
+      <c r="EA39" s="1"/>
+      <c r="EB39" s="1"/>
+      <c r="EC39" s="1"/>
+      <c r="ED39" s="1"/>
+      <c r="EE39" s="1"/>
+      <c r="EF39" s="1"/>
+      <c r="EG39" s="1"/>
+      <c r="EH39" s="1"/>
+      <c r="EI39" s="1"/>
+      <c r="EJ39" s="1"/>
+      <c r="EK39" s="1"/>
+      <c r="EL39" s="1"/>
+      <c r="EM39" s="1"/>
+      <c r="EN39" s="1"/>
+      <c r="EO39" s="1"/>
+      <c r="EP39" s="1"/>
+      <c r="EQ39" s="1"/>
+      <c r="ER39" s="1"/>
+      <c r="ES39" s="1"/>
+      <c r="ET39" s="1"/>
+      <c r="EU39" s="1"/>
+      <c r="EV39" s="1"/>
+      <c r="EW39" s="1"/>
+      <c r="EX39" s="1"/>
+      <c r="EY39" s="1"/>
+      <c r="EZ39" s="1"/>
+      <c r="FA39" s="1"/>
+      <c r="FB39" s="1"/>
+      <c r="FC39" s="1"/>
+      <c r="FD39" s="1"/>
+      <c r="FE39" s="1"/>
+      <c r="FF39" s="1"/>
+      <c r="FG39" s="1"/>
+      <c r="FH39" s="1"/>
+      <c r="FI39" s="1"/>
+      <c r="FJ39" s="1"/>
+      <c r="FK39" s="1"/>
+      <c r="FL39" s="1"/>
+      <c r="FM39" s="1"/>
+      <c r="FN39" s="1"/>
+      <c r="FO39" s="1"/>
+      <c r="FP39" s="1"/>
+      <c r="FQ39" s="1"/>
+      <c r="FR39" s="1"/>
+      <c r="FS39" s="1"/>
+      <c r="FT39" s="1"/>
+      <c r="FU39" s="1"/>
+      <c r="FV39" s="1"/>
+      <c r="FW39" s="1"/>
+      <c r="FX39" s="1"/>
+      <c r="FY39" s="1"/>
+      <c r="FZ39" s="1"/>
+      <c r="GA39" s="1"/>
+      <c r="GB39" s="1"/>
+      <c r="GC39" s="1"/>
+      <c r="GD39" s="1"/>
+      <c r="GE39" s="1"/>
+      <c r="GF39" s="1"/>
+      <c r="GG39" s="1"/>
+      <c r="GH39" s="1"/>
+      <c r="GI39" s="1"/>
+      <c r="GJ39" s="1"/>
+      <c r="GK39" s="1"/>
+      <c r="GL39" s="1"/>
+      <c r="GM39" s="1"/>
+      <c r="GN39" s="1"/>
+      <c r="GO39" s="1"/>
+      <c r="GP39" s="1"/>
+      <c r="GQ39" s="1"/>
+      <c r="GR39" s="1"/>
+      <c r="GS39" s="1"/>
+      <c r="GT39" s="1"/>
+      <c r="GU39" s="1"/>
+      <c r="GV39" s="1"/>
+      <c r="GW39" s="1"/>
+      <c r="GX39" s="1"/>
+      <c r="GY39" s="1"/>
+      <c r="GZ39" s="1"/>
+      <c r="HA39" s="1"/>
+      <c r="HB39" s="1"/>
+      <c r="HC39" s="1"/>
+      <c r="HD39" s="1"/>
+      <c r="HE39" s="1"/>
+      <c r="HF39" s="1"/>
+      <c r="HG39" s="1"/>
+      <c r="HH39" s="1"/>
+      <c r="HI39" s="1"/>
+      <c r="HJ39" s="1"/>
+      <c r="HK39" s="1"/>
+      <c r="HL39" s="1"/>
+      <c r="HM39" s="1"/>
+      <c r="HN39" s="1"/>
+      <c r="HO39" s="1"/>
+      <c r="HP39" s="1"/>
+      <c r="HQ39" s="1"/>
+      <c r="HR39" s="1"/>
+      <c r="HS39" s="1"/>
+      <c r="HT39" s="1"/>
+      <c r="HU39" s="1"/>
+      <c r="HV39" s="1"/>
+      <c r="HW39" s="1"/>
+      <c r="HX39" s="1"/>
+      <c r="HY39" s="1"/>
+      <c r="HZ39" s="1"/>
+      <c r="IA39" s="1"/>
+      <c r="IB39" s="1"/>
+      <c r="IC39" s="1"/>
+      <c r="ID39" s="1"/>
+      <c r="IE39" s="1"/>
+      <c r="IF39" s="1"/>
+      <c r="IG39" s="1"/>
+      <c r="IH39" s="1"/>
+      <c r="II39" s="1"/>
+      <c r="IJ39" s="1"/>
+      <c r="IK39" s="1"/>
+      <c r="IL39" s="1"/>
+      <c r="IM39" s="1"/>
+      <c r="IN39" s="1"/>
+      <c r="IO39" s="1"/>
+      <c r="IP39" s="1"/>
+      <c r="IQ39" s="1"/>
+      <c r="IR39" s="1"/>
+      <c r="IS39" s="1"/>
+      <c r="IT39" s="1"/>
+      <c r="IU39" s="1"/>
+      <c r="IV39" s="1"/>
+      <c r="IW39" s="1"/>
+      <c r="IX39" s="1"/>
+      <c r="IY39" s="1"/>
+      <c r="IZ39" s="1"/>
+      <c r="JA39" s="1"/>
+      <c r="JB39" s="1"/>
+      <c r="JC39" s="1"/>
+      <c r="JD39" s="1"/>
+      <c r="JE39" s="1"/>
+      <c r="JF39" s="1"/>
+      <c r="JG39" s="1"/>
+      <c r="JH39" s="1"/>
+      <c r="JI39" s="1"/>
+      <c r="JJ39" s="1"/>
+      <c r="JK39" s="1"/>
+      <c r="JL39" s="1"/>
+      <c r="JM39" s="1"/>
+      <c r="JN39" s="1"/>
+      <c r="JO39" s="1"/>
+    </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:S37" etc:filterBottomFollowUsedRange="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:S39" etc:filterBottomFollowUsedRange="0">
+    <filterColumn colId="15">
+      <filters>
+        <filter val="△"/>
+        <filter val="×"/>
+        <filter val="√"/>
+        <filter val="ok"/>
+        <filter val="○"/>
+      </filters>
+    </filterColumn>
+    <sortState ref="A2:S39">
+      <sortCondition ref="M1"/>
+    </sortState>
     <extLst/>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="L23" r:id="rId1" display="Cognitive, Affective, &amp; Behavioral Neuroscience" tooltip="https://link.springer.com/journal/13415"/>
-    <hyperlink ref="H31" r:id="rId2" display="merryndconstable@gmail.com"/>
-    <hyperlink ref="H2" r:id="rId2" display="merryndconstable@gmail.com" tooltip="mailto:merryndconstable@gmail.com"/>
-    <hyperlink ref="H30" r:id="rId3" display="hcp4715@gmail.com"/>
-    <hyperlink ref="H4" r:id="rId2" display="merryndconstable@gmail.com" tooltip="mailto:merryndconstable@gmail.com"/>
-    <hyperlink ref="H5" r:id="rId4" display="gaoxp@shnu.edu.cn" tooltip="mailto:gaoxp@shnu.edu.cn"/>
-    <hyperlink ref="H6" r:id="rId5" display="schaefer@psychologie-forum-muenster.de" tooltip="mailto:schaefer@psychologie-forum-muenster.de"/>
-    <hyperlink ref="H7" r:id="rId6" display="mgwozniak@gmail.com" tooltip="mailto:mgwozniak@gmail.com"/>
-    <hyperlink ref="H29" r:id="rId7" display="skumar@brookes.ac.uk"/>
-    <hyperlink ref="H24" r:id="rId8" display="marius.golubickis@abdn.ac.uk" tooltip="mailto:marius.golubickis@abdn.ac.uk"/>
-    <hyperlink ref="H8" r:id="rId9" display="mayanna@post.bgu.ac.il" tooltip="mailto:mayanna@post.bgu.ac.il"/>
-    <hyperlink ref="H37" r:id="rId10" display="gabyorellanac@gmail.com" tooltip="mailto:gabyorellanac@gmail.com"/>
+    <hyperlink ref="L2" r:id="rId1" display="Cognitive, Affective, &amp; Behavioral Neuroscience" tooltip="https://link.springer.com/journal/13415"/>
+    <hyperlink ref="H4" r:id="rId2" display="merryndconstable@gmail.com"/>
+    <hyperlink ref="H5" r:id="rId2" display="merryndconstable@gmail.com" tooltip="mailto:merryndconstable@gmail.com"/>
+    <hyperlink ref="H35" r:id="rId3" display="hcp4715@gmail.com"/>
+    <hyperlink ref="H6" r:id="rId2" display="merryndconstable@gmail.com" tooltip="mailto:merryndconstable@gmail.com"/>
+    <hyperlink ref="H20" r:id="rId4" display="gaoxp@shnu.edu.cn" tooltip="mailto:gaoxp@shnu.edu.cn"/>
+    <hyperlink ref="H21" r:id="rId5" display="schaefer@psychologie-forum-muenster.de" tooltip="mailto:schaefer@psychologie-forum-muenster.de"/>
+    <hyperlink ref="H27" r:id="rId6" display="mgwozniak@gmail.com" tooltip="mailto:mgwozniak@gmail.com"/>
+    <hyperlink ref="H34" r:id="rId7" display="skumar@brookes.ac.uk"/>
+    <hyperlink ref="H9" r:id="rId8" display="marius.golubickis@abdn.ac.uk" tooltip="mailto:marius.golubickis@abdn.ac.uk"/>
+    <hyperlink ref="H17" r:id="rId9" display="mayanna@post.bgu.ac.il" tooltip="mailto:mayanna@post.bgu.ac.il"/>
+    <hyperlink ref="H18" r:id="rId10" display="gabyorellanac@gmail.com" tooltip="mailto:gabyorellanac@gmail.com"/>
     <hyperlink ref="H12" r:id="rId3" display="hcp4715@gmail.com"/>
-    <hyperlink ref="H19" r:id="rId11" display="wf3126@mail.tsinghua.edu.cn" tooltip="mailto:wf3126@mail.tsinghua.edu.cn"/>
-    <hyperlink ref="H21" r:id="rId12" display="jie.sui@abdn.ac.uk"/>
-    <hyperlink ref="H22" r:id="rId13" display="lfuentes@um.es" tooltip="mailto:lfuentes@um.es"/>
-    <hyperlink ref="H34" r:id="rId14" display="tseng@riec.tohoku.ac.jp"/>
-    <hyperlink ref="H33" r:id="rId15" display="wentura@mx.uni-saarland.de" tooltip="mailto:wentura@mx.uni-saarland.de"/>
-    <hyperlink ref="H35" r:id="rId16" display="marcel.pauly@uni-saarlande.de"/>
-    <hyperlink ref="H32" r:id="rId17" display="mario.dalmaso@unipd.it"/>
-    <hyperlink ref="H36" r:id="rId18" display="jie.sui@psy.ox.ac.uk"/>
-    <hyperlink ref="I31" r:id="rId19" display="https://osf.io/sejw7/"/>
-    <hyperlink ref="I2" r:id="rId20" display="https://osf.io/5zaej/"/>
-    <hyperlink ref="I30" r:id="rId21" display="https://osf.io/4zvkm/"/>
-    <hyperlink ref="I29" r:id="rId22" display="https://figshare.com/s/e1391ebe3f11e8d70d9f" tooltip="https://figshare.com/s/e1391ebe3f11e8d70d9f"/>
-    <hyperlink ref="I4" r:id="rId23" display="https://osf.io/khyjq/"/>
-    <hyperlink ref="I5" r:id="rId24" display="https://osf.io/bw27c"/>
-    <hyperlink ref="I6" r:id="rId25" display="http://dx.doi.org/10.23668/psycharchives.2642"/>
-    <hyperlink ref="I7" r:id="rId26" display="https://journals.plos.org/plosone/article?id=10.1371/journal.pone.0190679#sec025"/>
-    <hyperlink ref="I24" r:id="rId27" display="https://osf.io/8bktn/" tooltip="https://osf.io/8bktn/"/>
-    <hyperlink ref="I8" r:id="rId28" display="https://osf.io/4srhn/?view_only=70ea4888bf524b598b0d61d04a54d9d9"/>
-    <hyperlink ref="I37" r:id="rId29" display="https://osf.io/3ke4f/" tooltip="https://osf.io/3ke4f/"/>
-    <hyperlink ref="I9" r:id="rId30" display="https://osf.io/cj7fp/"/>
-    <hyperlink ref="I11" r:id="rId31" display="https://osf.io/4n6j7/"/>
+    <hyperlink ref="H31" r:id="rId11" display="wf3126@mail.tsinghua.edu.cn" tooltip="mailto:wf3126@mail.tsinghua.edu.cn"/>
+    <hyperlink ref="H22" r:id="rId12" display="jie.sui@abdn.ac.uk"/>
+    <hyperlink ref="H16" r:id="rId13" display="lfuentes@um.es" tooltip="mailto:lfuentes@um.es"/>
+    <hyperlink ref="H37" r:id="rId14" display="tseng@riec.tohoku.ac.jp"/>
+    <hyperlink ref="H36" r:id="rId15" display="wentura@mx.uni-saarland.de" tooltip="mailto:wentura@mx.uni-saarland.de"/>
+    <hyperlink ref="H38" r:id="rId16" display="marcel.pauly@uni-saarlande.de"/>
+    <hyperlink ref="H7" r:id="rId17" display="mario.dalmaso@unipd.it"/>
+    <hyperlink ref="H39" r:id="rId18" display="jie.sui@psy.ox.ac.uk"/>
+    <hyperlink ref="I4" r:id="rId19" display="https://osf.io/sejw7/"/>
+    <hyperlink ref="I5" r:id="rId20" display="https://osf.io/5zaej/"/>
+    <hyperlink ref="I35" r:id="rId21" display="https://osf.io/4zvkm/"/>
+    <hyperlink ref="I34" r:id="rId22" display="https://figshare.com/s/e1391ebe3f11e8d70d9f" tooltip="https://figshare.com/s/e1391ebe3f11e8d70d9f"/>
+    <hyperlink ref="I6" r:id="rId23" display="https://osf.io/khyjq/"/>
+    <hyperlink ref="I20" r:id="rId24" display="https://osf.io/bw27c"/>
+    <hyperlink ref="I21" r:id="rId25" display="http://dx.doi.org/10.23668/psycharchives.2642"/>
+    <hyperlink ref="I27" r:id="rId26" display="https://journals.plos.org/plosone/article?id=10.1371/journal.pone.0190679#sec025"/>
+    <hyperlink ref="I9" r:id="rId27" display="https://osf.io/8bktn/" tooltip="https://osf.io/8bktn/"/>
+    <hyperlink ref="I17" r:id="rId28" display="https://osf.io/4srhn/?view_only=70ea4888bf524b598b0d61d04a54d9d9"/>
+    <hyperlink ref="I18" r:id="rId29" display="https://osf.io/3ke4f/" tooltip="https://osf.io/3ke4f/"/>
+    <hyperlink ref="I25" r:id="rId30" display="https://osf.io/cj7fp/"/>
+    <hyperlink ref="I15" r:id="rId31" display="https://osf.io/4n6j7/"/>
     <hyperlink ref="I12" r:id="rId32" display="https://zenodo.org/records/8031086"/>
-    <hyperlink ref="I13" r:id="rId33" display="https://osf.io/2juxk/?view_only=b4e01124337a4801b4beb99dbe803b8d"/>
-    <hyperlink ref="I14" r:id="rId34" display="https://researchdata.bath.ac.uk/924/" tooltip="https://researchdata.bath.ac.uk/924/"/>
-    <hyperlink ref="I15" r:id="rId35" display="https://osf.io/u9ty6/?view_only=9bdbbaf95f9a4d9c8bc53dd1a29563ae."/>
-    <hyperlink ref="I16" r:id="rId36" display="https://doi.org/10.17605/OSF.IO/FE3JW"/>
-    <hyperlink ref="I17" r:id="rId37" display="https://doi.org/10.26180/20011142"/>
-    <hyperlink ref="I18" r:id="rId38" display="https://osf.io/35wp9"/>
-    <hyperlink ref="I19" r:id="rId39" display="https://osf.io/hbrus/?view_only=98b2095f72e64fd382fc0d33de3f4497"/>
-    <hyperlink ref="I22" r:id="rId40" display="https://osf.io/tsvxy/?view_only=4314d303addf4dff9f443bea774a465a" tooltip="https://osf.io/tsvxy/?view_only=4314d303addf4dff9f443bea774a465a"/>
-    <hyperlink ref="H3" r:id="rId41" display="i.r.kolvoort@uva.nl" tooltip="mailto:i.r.kolvoort@uva.nl"/>
-    <hyperlink ref="H9" r:id="rId42" display="s.svensson.19@abdn.ac.uk"/>
-    <hyperlink ref="H13" r:id="rId43" display="pastoetter@uni-trier.de" tooltip="mailto:pastoetter@uni-trier.de"/>
-    <hyperlink ref="H14" r:id="rId44" display="c.hobbs@bristol.ac.uk;" tooltip="mailto:c.hobbs@bristol.ac.uk;"/>
-    <hyperlink ref="H16" r:id="rId45" display="michele.vicovaro@unipd.it"/>
-    <hyperlink ref="H17" r:id="rId46" display="kelsey.perrykkad@monash.edu"/>
-    <hyperlink ref="H18" r:id="rId6" display="mgwozniak@gmail.com" tooltip="mailto:mgwozniak@gmail.com"/>
-    <hyperlink ref="H23" r:id="rId47" display="letizia.amodeo@ugent.be"/>
-    <hyperlink ref="H26" r:id="rId48" display="victor.martinez5@um.es" tooltip="mailto:victor.martinez5@um.es"/>
-    <hyperlink ref="H25" r:id="rId49" display="hbbukowski@gmail.com"/>
-    <hyperlink ref="H20" r:id="rId50" display="hongjl18@mails.tsinghua.edu.cn" tooltip="mailto:hongjl18@mails.tsinghua.edu.cn"/>
-    <hyperlink ref="H10" r:id="rId51" display="guanll353@nenu.edu.cn"/>
-    <hyperlink ref="I27" r:id="rId52" display="https://osf.io/2q9w7/" tooltip="https://osf.io/2q9w7/"/>
-    <hyperlink ref="I26" r:id="rId53" display="https://www.frontiersin.org/journals/neuroscience/articles/10.3389/fnins.2020.00683/full" tooltip="https://www.frontiersin.org/journals/neuroscience/articles/10.3389/fnins.2020.00683/full"/>
-    <hyperlink ref="I25" r:id="rId54" display="https://osf.io/pcv3u/"/>
+    <hyperlink ref="I10" r:id="rId33" display="https://osf.io/2juxk/?view_only=b4e01124337a4801b4beb99dbe803b8d"/>
+    <hyperlink ref="I11" r:id="rId34" display="https://researchdata.bath.ac.uk/924/" tooltip="https://researchdata.bath.ac.uk/924/"/>
+    <hyperlink ref="I14" r:id="rId35" display="https://osf.io/u9ty6/?view_only=9bdbbaf95f9a4d9c8bc53dd1a29563ae."/>
+    <hyperlink ref="I26" r:id="rId36" display="https://doi.org/10.17605/OSF.IO/FE3JW"/>
+    <hyperlink ref="I19" r:id="rId37" display="https://doi.org/10.26180/20011142"/>
+    <hyperlink ref="I29" r:id="rId38" display="https://osf.io/35wp9"/>
+    <hyperlink ref="I31" r:id="rId39" display="https://osf.io/hbrus/?view_only=98b2095f72e64fd382fc0d33de3f4497"/>
+    <hyperlink ref="I16" r:id="rId40" display="https://osf.io/tsvxy/?view_only=4314d303addf4dff9f443bea774a465a" tooltip="https://osf.io/tsvxy/?view_only=4314d303addf4dff9f443bea774a465a"/>
+    <hyperlink ref="H13" r:id="rId41" display="i.r.kolvoort@uva.nl" tooltip="mailto:i.r.kolvoort@uva.nl"/>
+    <hyperlink ref="H25" r:id="rId42" display="s.svensson.19@abdn.ac.uk"/>
+    <hyperlink ref="H10" r:id="rId43" display="pastoetter@uni-trier.de" tooltip="mailto:pastoetter@uni-trier.de"/>
+    <hyperlink ref="H11" r:id="rId44" display="c.hobbs@bristol.ac.uk;" tooltip="mailto:c.hobbs@bristol.ac.uk;"/>
+    <hyperlink ref="H26" r:id="rId45" display="michele.vicovaro@unipd.it"/>
+    <hyperlink ref="H19" r:id="rId46" display="kelsey.perrykkad@monash.edu"/>
+    <hyperlink ref="H29" r:id="rId6" display="mgwozniak@gmail.com" tooltip="mailto:mgwozniak@gmail.com"/>
+    <hyperlink ref="H2" r:id="rId47" display="letizia.amodeo@ugent.be"/>
+    <hyperlink ref="H32" r:id="rId48" display="victor.martinez5@um.es" tooltip="mailto:victor.martinez5@um.es"/>
+    <hyperlink ref="H3" r:id="rId49" display="hbbukowski@gmail.com"/>
+    <hyperlink ref="H8" r:id="rId50" display="hongjl18@mails.tsinghua.edu.cn" tooltip="mailto:hongjl18@mails.tsinghua.edu.cn"/>
+    <hyperlink ref="H30" r:id="rId51" display="guanll353@nenu.edu.cn"/>
+    <hyperlink ref="I28" r:id="rId52" display="https://osf.io/2q9w7/" tooltip="https://osf.io/2q9w7/"/>
+    <hyperlink ref="I32" r:id="rId53" display="https://www.frontiersin.org/journals/neuroscience/articles/10.3389/fnins.2020.00683/full" tooltip="https://www.frontiersin.org/journals/neuroscience/articles/10.3389/fnins.2020.00683/full"/>
+    <hyperlink ref="I3" r:id="rId54" display="https://osf.io/pcv3u/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>